<commit_message>
fix wrong cel refs
</commit_message>
<xml_diff>
--- a/inst/template/populaiton_report_template_0001.xlsx
+++ b/inst/template/populaiton_report_template_0001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ms201\Desktop\大阪人口データの研究\create_excel\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBEEA6A-B3E2-4ECE-9981-63A4CE2A15C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23ECBAF4-E42B-41EF-92C0-44FF52C66241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="237">
   <si>
     <t>日付</t>
     <rPh sb="0" eb="2">
@@ -1574,16 +1574,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>過去五年増減</t>
-    <rPh sb="0" eb="4">
-      <t>カコゴネン</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ゾウゲン</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>過去５年増減</t>
     <rPh sb="0" eb="2">
       <t>カコ</t>
@@ -1670,6 +1660,16 @@
     </rPh>
     <rPh sb="5" eb="7">
       <t>ゾウゲン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>住民台帳</t>
+    <rPh sb="0" eb="2">
+      <t>ジュウミン</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ダイチョウ</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -2297,16 +2297,265 @@
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="8" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="8" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="183" fontId="7" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="183" fontId="7" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="8" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="8" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="183" fontId="7" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="183" fontId="7" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="8" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="8" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="183" fontId="7" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="183" fontId="7" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="180" fontId="14" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="10" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="14" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="180" fontId="14" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="14" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="14" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="182" fontId="16" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2324,14 +2573,38 @@
     <xf numFmtId="181" fontId="14" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="178" fontId="14" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="14" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="181" fontId="14" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="178" fontId="14" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="14" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="178" fontId="14" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
@@ -2388,15 +2661,6 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="176" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2468,275 +2732,11 @@
     <xf numFmtId="178" fontId="0" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="14" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="14" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="10" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="183" fontId="7" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="183" fontId="7" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="183" fontId="7" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="183" fontId="7" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="183" fontId="7" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="183" fontId="7" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="8" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="8" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="8" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="8" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="8" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="8" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5835,9 +5835,13 @@
     </a:p>
   </c:txPr>
   <c:printSettings>
-    <c:headerFooter/>
+    <c:headerFooter>
+      <c:oddFooter>&amp;Rデータ出典「大阪府の毎月推計人口」
+https://www.pref.osaka.lg.jp/o040090/toukei/jinkou/index.html
+</c:oddFooter>
+    </c:headerFooter>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -17491,62 +17495,57 @@
   <dimension ref="A1:BF67"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AP2" sqref="AP2"/>
-      <extLst>
-        <ext xmlns:xlsdti="http://schemas.microsoft.com/office/spreadsheetml/2023/showDataTypeIcons" uri="{77bfe23e-c014-4d31-8a63-9c772dbf06b6}">
-          <xlsdti:showDataTypeIcons visible="0"/>
-        </ext>
-      </extLst>
+      <selection activeCell="A5" sqref="A5:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="18.75"/>
   <sheetData>
     <row r="1" spans="1:58" ht="18.75" customHeight="1">
-      <c r="A1" s="49" t="str">
+      <c r="A1" s="140" t="str">
         <f>(source!B2)</f>
         <v>大阪市福島区</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
+      <c r="F1" s="140"/>
+      <c r="G1" s="140"/>
+      <c r="H1" s="140"/>
+      <c r="I1" s="140"/>
+      <c r="J1" s="140"/>
+      <c r="K1" s="140"/>
+      <c r="L1" s="140"/>
+      <c r="M1" s="140"/>
+      <c r="N1" s="140"/>
+      <c r="O1" s="140"/>
+      <c r="P1" s="140"/>
       <c r="Q1" s="27"/>
       <c r="R1" s="27"/>
-      <c r="S1" s="176" t="s">
-        <v>234</v>
-      </c>
-      <c r="T1" s="176"/>
-      <c r="U1" s="176"/>
-      <c r="V1" s="176"/>
-      <c r="W1" s="176"/>
-      <c r="X1" s="176"/>
-      <c r="Y1" s="176"/>
-      <c r="Z1" s="176"/>
-      <c r="AA1" s="176"/>
-      <c r="AB1" s="176"/>
-      <c r="AC1" s="176"/>
-      <c r="AD1" s="176"/>
-      <c r="AE1" s="176"/>
-      <c r="AF1" s="176"/>
-      <c r="AG1" s="176"/>
-      <c r="AH1" s="176"/>
-      <c r="AI1" s="176"/>
-      <c r="AJ1" s="176"/>
-      <c r="AK1" s="176"/>
-      <c r="AL1" s="176"/>
-      <c r="AM1" s="176"/>
-      <c r="AN1" s="176"/>
+      <c r="S1" s="38" t="s">
+        <v>233</v>
+      </c>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="38"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="38"/>
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="38"/>
+      <c r="AN1" s="38"/>
       <c r="AO1" s="27"/>
       <c r="AP1" s="27"/>
       <c r="AQ1" s="27"/>
@@ -17555,63 +17554,63 @@
       <c r="AT1" s="27"/>
       <c r="AU1" s="27"/>
       <c r="AV1" s="27"/>
-      <c r="AW1" s="38" t="s">
-        <v>235</v>
-      </c>
-      <c r="AX1" s="38"/>
-      <c r="AY1" s="38"/>
-      <c r="AZ1" s="38"/>
-      <c r="BA1" s="38"/>
-      <c r="BB1" s="37">
+      <c r="AW1" s="139" t="s">
+        <v>234</v>
+      </c>
+      <c r="AX1" s="139"/>
+      <c r="AY1" s="139"/>
+      <c r="AZ1" s="139"/>
+      <c r="BA1" s="139"/>
+      <c r="BB1" s="138">
         <f>(t_data!B59)</f>
         <v>0</v>
       </c>
-      <c r="BC1" s="37"/>
-      <c r="BD1" s="37"/>
-      <c r="BE1" s="37"/>
-      <c r="BF1" s="37"/>
+      <c r="BC1" s="138"/>
+      <c r="BD1" s="138"/>
+      <c r="BE1" s="138"/>
+      <c r="BF1" s="138"/>
     </row>
     <row r="2" spans="1:58" ht="18.75" customHeight="1">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
+      <c r="A2" s="140"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="140"/>
+      <c r="L2" s="140"/>
+      <c r="M2" s="140"/>
+      <c r="N2" s="140"/>
+      <c r="O2" s="140"/>
+      <c r="P2" s="140"/>
       <c r="Q2" s="27"/>
       <c r="R2" s="27"/>
-      <c r="S2" s="176"/>
-      <c r="T2" s="176"/>
-      <c r="U2" s="176"/>
-      <c r="V2" s="176"/>
-      <c r="W2" s="176"/>
-      <c r="X2" s="176"/>
-      <c r="Y2" s="176"/>
-      <c r="Z2" s="176"/>
-      <c r="AA2" s="176"/>
-      <c r="AB2" s="176"/>
-      <c r="AC2" s="176"/>
-      <c r="AD2" s="176"/>
-      <c r="AE2" s="176"/>
-      <c r="AF2" s="176"/>
-      <c r="AG2" s="176"/>
-      <c r="AH2" s="176"/>
-      <c r="AI2" s="176"/>
-      <c r="AJ2" s="176"/>
-      <c r="AK2" s="176"/>
-      <c r="AL2" s="176"/>
-      <c r="AM2" s="176"/>
-      <c r="AN2" s="176"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="38"/>
+      <c r="AH2" s="38"/>
+      <c r="AI2" s="38"/>
+      <c r="AJ2" s="38"/>
+      <c r="AK2" s="38"/>
+      <c r="AL2" s="38"/>
+      <c r="AM2" s="38"/>
+      <c r="AN2" s="38"/>
       <c r="AO2" s="27"/>
       <c r="AP2" s="27"/>
       <c r="AQ2" s="27"/>
@@ -17632,624 +17631,624 @@
       <c r="BF2" s="27"/>
     </row>
     <row r="3" spans="1:58" ht="18.75" customHeight="1">
-      <c r="A3" s="114" t="s">
+      <c r="A3" s="183" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="114"/>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="114"/>
-      <c r="K3" s="114"/>
-      <c r="L3" s="114"/>
-      <c r="M3" s="114"/>
-      <c r="N3" s="114"/>
-      <c r="O3" s="114"/>
-      <c r="P3" s="114"/>
-      <c r="Q3" s="114"/>
-      <c r="R3" s="114"/>
-      <c r="S3" s="114"/>
-      <c r="T3" s="114"/>
-      <c r="U3" s="114"/>
-      <c r="V3" s="114"/>
-      <c r="W3" s="114"/>
-      <c r="X3" s="114"/>
-      <c r="Y3" s="114"/>
-      <c r="Z3" s="114"/>
-      <c r="AA3" s="114"/>
-      <c r="AB3" s="114"/>
-      <c r="AC3" s="114"/>
-      <c r="AD3" s="114"/>
-      <c r="AE3" s="114"/>
-      <c r="AF3" s="114"/>
-      <c r="AG3" s="114"/>
-      <c r="AH3" s="114"/>
-      <c r="AI3" s="114"/>
-      <c r="AJ3" s="114"/>
-      <c r="AK3" s="114"/>
-      <c r="AL3" s="114"/>
-      <c r="AM3" s="114"/>
-      <c r="AN3" s="114"/>
-      <c r="AO3" s="114"/>
-      <c r="AP3" s="114"/>
-      <c r="AQ3" s="114"/>
-      <c r="AR3" s="114"/>
-      <c r="AS3" s="114"/>
-      <c r="AT3" s="114"/>
-      <c r="AU3" s="114"/>
-      <c r="AV3" s="114"/>
-      <c r="AW3" s="114"/>
-      <c r="AX3" s="114"/>
-      <c r="AY3" s="114"/>
-      <c r="AZ3" s="17"/>
-      <c r="BA3" s="17"/>
-      <c r="BB3" s="17"/>
-      <c r="BC3" s="17"/>
-      <c r="BD3" s="17"/>
-      <c r="BE3" s="17"/>
-      <c r="BF3" s="17"/>
+      <c r="B3" s="183"/>
+      <c r="C3" s="183"/>
+      <c r="D3" s="183"/>
+      <c r="E3" s="183"/>
+      <c r="F3" s="183"/>
+      <c r="G3" s="183"/>
+      <c r="H3" s="183"/>
+      <c r="I3" s="183"/>
+      <c r="J3" s="183"/>
+      <c r="K3" s="183"/>
+      <c r="L3" s="183"/>
+      <c r="M3" s="183"/>
+      <c r="N3" s="183"/>
+      <c r="O3" s="183"/>
+      <c r="P3" s="183"/>
+      <c r="Q3" s="183"/>
+      <c r="R3" s="183"/>
+      <c r="S3" s="183"/>
+      <c r="T3" s="183"/>
+      <c r="U3" s="183"/>
+      <c r="V3" s="183"/>
+      <c r="W3" s="183"/>
+      <c r="X3" s="183"/>
+      <c r="Y3" s="183"/>
+      <c r="Z3" s="183"/>
+      <c r="AA3" s="183"/>
+      <c r="AB3" s="183"/>
+      <c r="AC3" s="183"/>
+      <c r="AD3" s="183"/>
+      <c r="AE3" s="183"/>
+      <c r="AF3" s="183"/>
+      <c r="AG3" s="183"/>
+      <c r="AH3" s="183"/>
+      <c r="AI3" s="183"/>
+      <c r="AJ3" s="183"/>
+      <c r="AK3" s="183"/>
+      <c r="AL3" s="183"/>
+      <c r="AM3" s="183"/>
+      <c r="AN3" s="183"/>
+      <c r="AO3" s="183"/>
+      <c r="AP3" s="183"/>
+      <c r="AQ3" s="183"/>
+      <c r="AR3" s="183"/>
+      <c r="AS3" s="183"/>
+      <c r="AT3" s="183"/>
+      <c r="AU3" s="183"/>
+      <c r="AV3" s="183"/>
+      <c r="AW3" s="183"/>
+      <c r="AX3" s="183"/>
+      <c r="AY3" s="183"/>
+      <c r="AZ3" s="27"/>
+      <c r="BA3" s="27"/>
+      <c r="BB3" s="27"/>
+      <c r="BC3" s="27"/>
+      <c r="BD3" s="27"/>
+      <c r="BE3" s="27"/>
+      <c r="BF3" s="27"/>
     </row>
     <row r="4" spans="1:58">
-      <c r="A4" s="110"/>
-      <c r="B4" s="110"/>
-      <c r="C4" s="110"/>
-      <c r="D4" s="111" t="str">
+      <c r="A4" s="109"/>
+      <c r="B4" s="109"/>
+      <c r="C4" s="109"/>
+      <c r="D4" s="108" t="str">
         <f>(t_data!$B$5)</f>
         <v>2020-08-01</v>
       </c>
-      <c r="E4" s="110"/>
-      <c r="F4" s="110"/>
-      <c r="G4" s="110"/>
-      <c r="H4" s="110"/>
-      <c r="I4" s="110"/>
-      <c r="J4" s="110"/>
-      <c r="K4" s="110"/>
-      <c r="L4" s="111" t="str">
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="108" t="str">
         <f>(t_data!$B$6)</f>
         <v>2021-08-01</v>
       </c>
-      <c r="M4" s="110"/>
-      <c r="N4" s="110"/>
-      <c r="O4" s="110"/>
-      <c r="P4" s="110"/>
-      <c r="Q4" s="110"/>
-      <c r="R4" s="110"/>
-      <c r="S4" s="110"/>
-      <c r="T4" s="111" t="str">
+      <c r="M4" s="109"/>
+      <c r="N4" s="109"/>
+      <c r="O4" s="109"/>
+      <c r="P4" s="109"/>
+      <c r="Q4" s="109"/>
+      <c r="R4" s="109"/>
+      <c r="S4" s="109"/>
+      <c r="T4" s="108" t="str">
         <f>(t_data!$B$7)</f>
         <v>2022-08-01</v>
       </c>
-      <c r="U4" s="110"/>
-      <c r="V4" s="110"/>
-      <c r="W4" s="110"/>
-      <c r="X4" s="110"/>
-      <c r="Y4" s="110"/>
-      <c r="Z4" s="110"/>
-      <c r="AA4" s="110"/>
-      <c r="AB4" s="111" t="str">
+      <c r="U4" s="109"/>
+      <c r="V4" s="109"/>
+      <c r="W4" s="109"/>
+      <c r="X4" s="109"/>
+      <c r="Y4" s="109"/>
+      <c r="Z4" s="109"/>
+      <c r="AA4" s="109"/>
+      <c r="AB4" s="108" t="str">
         <f>(t_data!$B$8)</f>
         <v>2023-08-01</v>
       </c>
-      <c r="AC4" s="110"/>
-      <c r="AD4" s="110"/>
-      <c r="AE4" s="110"/>
-      <c r="AF4" s="110"/>
-      <c r="AG4" s="110"/>
-      <c r="AH4" s="110"/>
-      <c r="AI4" s="110"/>
-      <c r="AJ4" s="111" t="str">
+      <c r="AC4" s="109"/>
+      <c r="AD4" s="109"/>
+      <c r="AE4" s="109"/>
+      <c r="AF4" s="109"/>
+      <c r="AG4" s="109"/>
+      <c r="AH4" s="109"/>
+      <c r="AI4" s="109"/>
+      <c r="AJ4" s="108" t="str">
         <f>(t_data!$B$9)</f>
         <v>2024-08-01</v>
       </c>
-      <c r="AK4" s="110"/>
-      <c r="AL4" s="110"/>
-      <c r="AM4" s="110"/>
-      <c r="AN4" s="110"/>
-      <c r="AO4" s="110"/>
-      <c r="AP4" s="110"/>
-      <c r="AQ4" s="110"/>
-      <c r="AR4" s="111" t="str">
+      <c r="AK4" s="109"/>
+      <c r="AL4" s="109"/>
+      <c r="AM4" s="109"/>
+      <c r="AN4" s="109"/>
+      <c r="AO4" s="109"/>
+      <c r="AP4" s="109"/>
+      <c r="AQ4" s="109"/>
+      <c r="AR4" s="108" t="str">
         <f>(t_data!$B$10)</f>
         <v>2025-08-01</v>
       </c>
-      <c r="AS4" s="110"/>
-      <c r="AT4" s="110"/>
-      <c r="AU4" s="110"/>
-      <c r="AV4" s="110"/>
-      <c r="AW4" s="110"/>
-      <c r="AX4" s="110"/>
-      <c r="AY4" s="144"/>
-      <c r="AZ4" s="94" t="s">
+      <c r="AS4" s="109"/>
+      <c r="AT4" s="109"/>
+      <c r="AU4" s="109"/>
+      <c r="AV4" s="109"/>
+      <c r="AW4" s="109"/>
+      <c r="AX4" s="109"/>
+      <c r="AY4" s="110"/>
+      <c r="AZ4" s="133" t="s">
         <v>227</v>
       </c>
-      <c r="BA4" s="95"/>
-      <c r="BB4" s="95"/>
-      <c r="BC4" s="95"/>
-      <c r="BD4" s="95"/>
-      <c r="BE4" s="95"/>
-      <c r="BF4" s="96"/>
+      <c r="BA4" s="134"/>
+      <c r="BB4" s="134"/>
+      <c r="BC4" s="134"/>
+      <c r="BD4" s="134"/>
+      <c r="BE4" s="134"/>
+      <c r="BF4" s="135"/>
     </row>
     <row r="5" spans="1:58" ht="18.75" customHeight="1">
-      <c r="A5" s="112" t="s">
+      <c r="A5" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="112"/>
-      <c r="C5" s="112"/>
-      <c r="D5" s="106">
+      <c r="B5" s="119"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="111">
         <f>(t_data!$C$5)</f>
         <v>79271</v>
       </c>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="100">
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="115">
         <f>(t_data!$D$5)</f>
         <v>2122</v>
       </c>
-      <c r="J5" s="100"/>
-      <c r="K5" s="101"/>
-      <c r="L5" s="106">
+      <c r="J5" s="115"/>
+      <c r="K5" s="117"/>
+      <c r="L5" s="111">
         <f>(t_data!$C$6)</f>
         <v>79888</v>
       </c>
-      <c r="M5" s="107"/>
-      <c r="N5" s="107"/>
-      <c r="O5" s="107"/>
-      <c r="P5" s="107"/>
-      <c r="Q5" s="100">
+      <c r="M5" s="112"/>
+      <c r="N5" s="112"/>
+      <c r="O5" s="112"/>
+      <c r="P5" s="112"/>
+      <c r="Q5" s="115">
         <f>(t_data!$D$6)</f>
         <v>617</v>
       </c>
-      <c r="R5" s="100"/>
-      <c r="S5" s="101"/>
-      <c r="T5" s="106">
+      <c r="R5" s="115"/>
+      <c r="S5" s="117"/>
+      <c r="T5" s="111">
         <f>(t_data!$C$7)</f>
         <v>80135</v>
       </c>
-      <c r="U5" s="107"/>
-      <c r="V5" s="107"/>
-      <c r="W5" s="107"/>
-      <c r="X5" s="107"/>
-      <c r="Y5" s="100">
+      <c r="U5" s="112"/>
+      <c r="V5" s="112"/>
+      <c r="W5" s="112"/>
+      <c r="X5" s="112"/>
+      <c r="Y5" s="115">
         <f>(t_data!$D$7)</f>
         <v>247</v>
       </c>
-      <c r="Z5" s="100"/>
-      <c r="AA5" s="101"/>
-      <c r="AB5" s="106">
+      <c r="Z5" s="115"/>
+      <c r="AA5" s="117"/>
+      <c r="AB5" s="111">
         <f>(t_data!$C$8)</f>
         <v>81678</v>
       </c>
-      <c r="AC5" s="107"/>
-      <c r="AD5" s="107"/>
-      <c r="AE5" s="107"/>
-      <c r="AF5" s="107"/>
-      <c r="AG5" s="100">
+      <c r="AC5" s="112"/>
+      <c r="AD5" s="112"/>
+      <c r="AE5" s="112"/>
+      <c r="AF5" s="112"/>
+      <c r="AG5" s="115">
         <f>(t_data!$D$8)</f>
         <v>1543</v>
       </c>
-      <c r="AH5" s="100"/>
-      <c r="AI5" s="101"/>
-      <c r="AJ5" s="106">
+      <c r="AH5" s="115"/>
+      <c r="AI5" s="117"/>
+      <c r="AJ5" s="111">
         <f>(t_data!$C$9)</f>
         <v>83257</v>
       </c>
-      <c r="AK5" s="107"/>
-      <c r="AL5" s="107"/>
-      <c r="AM5" s="107"/>
-      <c r="AN5" s="107"/>
-      <c r="AO5" s="100">
+      <c r="AK5" s="112"/>
+      <c r="AL5" s="112"/>
+      <c r="AM5" s="112"/>
+      <c r="AN5" s="112"/>
+      <c r="AO5" s="115">
         <f>(t_data!$D$9)</f>
         <v>1579</v>
       </c>
-      <c r="AP5" s="100"/>
-      <c r="AQ5" s="101"/>
-      <c r="AR5" s="106">
+      <c r="AP5" s="115"/>
+      <c r="AQ5" s="117"/>
+      <c r="AR5" s="111">
         <f>(t_data!$C$10)</f>
         <v>83730</v>
       </c>
-      <c r="AS5" s="107"/>
-      <c r="AT5" s="107"/>
-      <c r="AU5" s="107"/>
-      <c r="AV5" s="107"/>
-      <c r="AW5" s="100">
+      <c r="AS5" s="112"/>
+      <c r="AT5" s="112"/>
+      <c r="AU5" s="112"/>
+      <c r="AV5" s="112"/>
+      <c r="AW5" s="115">
         <f>(t_data!$D$10)</f>
         <v>473</v>
       </c>
-      <c r="AX5" s="100"/>
-      <c r="AY5" s="100"/>
-      <c r="AZ5" s="74">
+      <c r="AX5" s="115"/>
+      <c r="AY5" s="115"/>
+      <c r="AZ5" s="162">
         <f>(t_data!D11)</f>
         <v>4459</v>
       </c>
-      <c r="BA5" s="75"/>
-      <c r="BB5" s="75"/>
-      <c r="BC5" s="75"/>
-      <c r="BD5" s="60">
+      <c r="BA5" s="163"/>
+      <c r="BB5" s="163"/>
+      <c r="BC5" s="163"/>
+      <c r="BD5" s="151">
         <f>(t_data!E11)</f>
         <v>5.6250078843461004E-2</v>
       </c>
-      <c r="BE5" s="60"/>
-      <c r="BF5" s="61"/>
+      <c r="BE5" s="151"/>
+      <c r="BF5" s="152"/>
     </row>
     <row r="6" spans="1:58" ht="18.75" customHeight="1">
-      <c r="A6" s="113"/>
-      <c r="B6" s="113"/>
-      <c r="C6" s="113"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="103">
+      <c r="A6" s="120"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="120"/>
+      <c r="D6" s="113"/>
+      <c r="E6" s="114"/>
+      <c r="F6" s="114"/>
+      <c r="G6" s="114"/>
+      <c r="H6" s="114"/>
+      <c r="I6" s="116">
         <f>(t_data!$E$5)</f>
         <v>2.7505217177150598E-2</v>
       </c>
-      <c r="J6" s="103"/>
-      <c r="K6" s="104"/>
-      <c r="L6" s="108"/>
-      <c r="M6" s="109"/>
-      <c r="N6" s="109"/>
-      <c r="O6" s="109"/>
-      <c r="P6" s="109"/>
-      <c r="Q6" s="103">
+      <c r="J6" s="116"/>
+      <c r="K6" s="118"/>
+      <c r="L6" s="113"/>
+      <c r="M6" s="114"/>
+      <c r="N6" s="114"/>
+      <c r="O6" s="114"/>
+      <c r="P6" s="114"/>
+      <c r="Q6" s="116">
         <f>(t_data!$E$6)</f>
         <v>7.7834264737419723E-3</v>
       </c>
-      <c r="R6" s="103"/>
-      <c r="S6" s="104"/>
-      <c r="T6" s="108"/>
-      <c r="U6" s="109"/>
-      <c r="V6" s="109"/>
-      <c r="W6" s="109"/>
-      <c r="X6" s="109"/>
-      <c r="Y6" s="103">
+      <c r="R6" s="116"/>
+      <c r="S6" s="118"/>
+      <c r="T6" s="113"/>
+      <c r="U6" s="114"/>
+      <c r="V6" s="114"/>
+      <c r="W6" s="114"/>
+      <c r="X6" s="114"/>
+      <c r="Y6" s="116">
         <f>(t_data!$E$7)</f>
         <v>3.0918285599839113E-3</v>
       </c>
-      <c r="Z6" s="103"/>
-      <c r="AA6" s="104"/>
-      <c r="AB6" s="108"/>
-      <c r="AC6" s="109"/>
-      <c r="AD6" s="109"/>
-      <c r="AE6" s="109"/>
-      <c r="AF6" s="109"/>
-      <c r="AG6" s="103">
+      <c r="Z6" s="116"/>
+      <c r="AA6" s="118"/>
+      <c r="AB6" s="113"/>
+      <c r="AC6" s="114"/>
+      <c r="AD6" s="114"/>
+      <c r="AE6" s="114"/>
+      <c r="AF6" s="114"/>
+      <c r="AG6" s="116">
         <f>(t_data!$E$8)</f>
         <v>1.9255007175391636E-2</v>
       </c>
-      <c r="AH6" s="103"/>
-      <c r="AI6" s="104"/>
-      <c r="AJ6" s="108"/>
-      <c r="AK6" s="109"/>
-      <c r="AL6" s="109"/>
-      <c r="AM6" s="109"/>
-      <c r="AN6" s="109"/>
-      <c r="AO6" s="103">
+      <c r="AH6" s="116"/>
+      <c r="AI6" s="118"/>
+      <c r="AJ6" s="113"/>
+      <c r="AK6" s="114"/>
+      <c r="AL6" s="114"/>
+      <c r="AM6" s="114"/>
+      <c r="AN6" s="114"/>
+      <c r="AO6" s="116">
         <f>(t_data!$E$9)</f>
         <v>1.9332011067851873E-2</v>
       </c>
-      <c r="AP6" s="103"/>
-      <c r="AQ6" s="104"/>
-      <c r="AR6" s="108"/>
-      <c r="AS6" s="109"/>
-      <c r="AT6" s="109"/>
-      <c r="AU6" s="109"/>
-      <c r="AV6" s="109"/>
-      <c r="AW6" s="103">
-        <f>(t_data!$E$9)</f>
-        <v>1.9332011067851873E-2</v>
-      </c>
-      <c r="AX6" s="103"/>
-      <c r="AY6" s="103"/>
+      <c r="AP6" s="116"/>
+      <c r="AQ6" s="118"/>
+      <c r="AR6" s="113"/>
+      <c r="AS6" s="114"/>
+      <c r="AT6" s="114"/>
+      <c r="AU6" s="114"/>
+      <c r="AV6" s="114"/>
+      <c r="AW6" s="116">
+        <f>(t_data!$E$10)</f>
+        <v>5.6812039828482153E-3</v>
+      </c>
+      <c r="AX6" s="116"/>
+      <c r="AY6" s="116"/>
       <c r="AZ6" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="BA6" s="67">
+      <c r="BA6" s="158">
         <f>(t_data!G11)</f>
         <v>2209</v>
       </c>
-      <c r="BB6" s="67"/>
-      <c r="BC6" s="67"/>
-      <c r="BD6" s="62">
+      <c r="BB6" s="158"/>
+      <c r="BC6" s="158"/>
+      <c r="BD6" s="153">
         <f>(t_data!H11)</f>
         <v>5.8782830836371369E-2</v>
       </c>
-      <c r="BE6" s="62"/>
-      <c r="BF6" s="63"/>
+      <c r="BE6" s="153"/>
+      <c r="BF6" s="154"/>
     </row>
     <row r="7" spans="1:58">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="136" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="102"/>
-      <c r="C7" s="102"/>
-      <c r="D7" s="98">
+      <c r="B7" s="136"/>
+      <c r="C7" s="136"/>
+      <c r="D7" s="121">
         <f>(t_data!$F$5)</f>
         <v>37579</v>
       </c>
-      <c r="E7" s="99"/>
-      <c r="F7" s="99"/>
-      <c r="G7" s="99"/>
-      <c r="H7" s="39">
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="123">
         <f>(t_data!$I$5)</f>
         <v>41692</v>
       </c>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="98">
+      <c r="I7" s="123"/>
+      <c r="J7" s="123"/>
+      <c r="K7" s="130"/>
+      <c r="L7" s="121">
         <f>(t_data!$F$6)</f>
         <v>37883</v>
       </c>
-      <c r="M7" s="99"/>
-      <c r="N7" s="99"/>
-      <c r="O7" s="99"/>
-      <c r="P7" s="39">
+      <c r="M7" s="122"/>
+      <c r="N7" s="122"/>
+      <c r="O7" s="122"/>
+      <c r="P7" s="123">
         <f>(t_data!$I$6)</f>
         <v>42005</v>
       </c>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="40"/>
-      <c r="T7" s="98">
+      <c r="Q7" s="123"/>
+      <c r="R7" s="123"/>
+      <c r="S7" s="130"/>
+      <c r="T7" s="121">
         <f>(t_data!$F$7)</f>
         <v>37943</v>
       </c>
-      <c r="U7" s="99"/>
-      <c r="V7" s="99"/>
-      <c r="W7" s="99"/>
-      <c r="X7" s="39">
+      <c r="U7" s="122"/>
+      <c r="V7" s="122"/>
+      <c r="W7" s="122"/>
+      <c r="X7" s="123">
         <f>(t_data!$I$7)</f>
         <v>42192</v>
       </c>
-      <c r="Y7" s="39"/>
-      <c r="Z7" s="39"/>
-      <c r="AA7" s="40"/>
-      <c r="AB7" s="98">
+      <c r="Y7" s="123"/>
+      <c r="Z7" s="123"/>
+      <c r="AA7" s="130"/>
+      <c r="AB7" s="121">
         <f>(t_data!$F$8)</f>
         <v>38675</v>
       </c>
-      <c r="AC7" s="99"/>
-      <c r="AD7" s="99"/>
-      <c r="AE7" s="99"/>
-      <c r="AF7" s="39">
+      <c r="AC7" s="122"/>
+      <c r="AD7" s="122"/>
+      <c r="AE7" s="122"/>
+      <c r="AF7" s="123">
         <f>(t_data!$I$8)</f>
         <v>43003</v>
       </c>
-      <c r="AG7" s="39"/>
-      <c r="AH7" s="39"/>
-      <c r="AI7" s="40"/>
-      <c r="AJ7" s="98">
+      <c r="AG7" s="123"/>
+      <c r="AH7" s="123"/>
+      <c r="AI7" s="130"/>
+      <c r="AJ7" s="121">
         <f>(t_data!$F$9)</f>
         <v>39492</v>
       </c>
-      <c r="AK7" s="99"/>
-      <c r="AL7" s="99"/>
-      <c r="AM7" s="99"/>
-      <c r="AN7" s="39">
+      <c r="AK7" s="122"/>
+      <c r="AL7" s="122"/>
+      <c r="AM7" s="122"/>
+      <c r="AN7" s="123">
         <f>(t_data!$I$9)</f>
         <v>43765</v>
       </c>
-      <c r="AO7" s="39"/>
-      <c r="AP7" s="39"/>
-      <c r="AQ7" s="40"/>
-      <c r="AR7" s="98">
+      <c r="AO7" s="123"/>
+      <c r="AP7" s="123"/>
+      <c r="AQ7" s="130"/>
+      <c r="AR7" s="121">
         <f>(t_data!$F$10)</f>
         <v>39788</v>
       </c>
-      <c r="AS7" s="99"/>
-      <c r="AT7" s="99"/>
-      <c r="AU7" s="99"/>
-      <c r="AV7" s="39">
+      <c r="AS7" s="122"/>
+      <c r="AT7" s="122"/>
+      <c r="AU7" s="122"/>
+      <c r="AV7" s="123">
         <f>(t_data!$I$10)</f>
         <v>43942</v>
       </c>
-      <c r="AW7" s="39"/>
-      <c r="AX7" s="39"/>
-      <c r="AY7" s="39"/>
+      <c r="AW7" s="123"/>
+      <c r="AX7" s="123"/>
+      <c r="AY7" s="123"/>
       <c r="AZ7" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="BA7" s="66">
+      <c r="BA7" s="157">
         <f>(t_data!J11)</f>
         <v>2250</v>
       </c>
-      <c r="BB7" s="66"/>
-      <c r="BC7" s="66"/>
-      <c r="BD7" s="64">
+      <c r="BB7" s="157"/>
+      <c r="BC7" s="157"/>
+      <c r="BD7" s="155">
         <f>(t_data!K11)</f>
         <v>5.3967187949726547E-2</v>
       </c>
-      <c r="BE7" s="64"/>
-      <c r="BF7" s="65"/>
+      <c r="BE7" s="155"/>
+      <c r="BF7" s="156"/>
     </row>
     <row r="8" spans="1:58" ht="18.75" customHeight="1">
-      <c r="A8" s="105" t="s">
+      <c r="A8" s="137" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="105"/>
-      <c r="C8" s="105"/>
-      <c r="D8" s="41">
+      <c r="B8" s="137"/>
+      <c r="C8" s="137"/>
+      <c r="D8" s="124">
         <f>(t_data!$L$5)</f>
         <v>42611</v>
       </c>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="45">
+      <c r="E8" s="125"/>
+      <c r="F8" s="125"/>
+      <c r="G8" s="125"/>
+      <c r="H8" s="125"/>
+      <c r="I8" s="128">
         <f>(t_data!$M$5)</f>
         <v>1309</v>
       </c>
-      <c r="J8" s="45"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="41">
+      <c r="J8" s="128"/>
+      <c r="K8" s="131"/>
+      <c r="L8" s="124">
         <f>(t_data!$L$6)</f>
         <v>43271</v>
       </c>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="45">
+      <c r="M8" s="125"/>
+      <c r="N8" s="125"/>
+      <c r="O8" s="125"/>
+      <c r="P8" s="125"/>
+      <c r="Q8" s="128">
         <f>(t_data!$M$6)</f>
         <v>660</v>
       </c>
-      <c r="R8" s="45"/>
-      <c r="S8" s="46"/>
-      <c r="T8" s="41">
+      <c r="R8" s="128"/>
+      <c r="S8" s="131"/>
+      <c r="T8" s="124">
         <f>(t_data!$L$7)</f>
         <v>43813</v>
       </c>
-      <c r="U8" s="42"/>
-      <c r="V8" s="42"/>
-      <c r="W8" s="42"/>
-      <c r="X8" s="42"/>
-      <c r="Y8" s="45">
+      <c r="U8" s="125"/>
+      <c r="V8" s="125"/>
+      <c r="W8" s="125"/>
+      <c r="X8" s="125"/>
+      <c r="Y8" s="128">
         <f>(t_data!$M$7)</f>
         <v>542</v>
       </c>
-      <c r="Z8" s="45"/>
-      <c r="AA8" s="46"/>
-      <c r="AB8" s="41">
+      <c r="Z8" s="128"/>
+      <c r="AA8" s="131"/>
+      <c r="AB8" s="124">
         <f>(t_data!$L$8)</f>
         <v>45127</v>
       </c>
-      <c r="AC8" s="42"/>
-      <c r="AD8" s="42"/>
-      <c r="AE8" s="42"/>
-      <c r="AF8" s="42"/>
-      <c r="AG8" s="45">
+      <c r="AC8" s="125"/>
+      <c r="AD8" s="125"/>
+      <c r="AE8" s="125"/>
+      <c r="AF8" s="125"/>
+      <c r="AG8" s="128">
         <f>(t_data!$M$8)</f>
         <v>1314</v>
       </c>
-      <c r="AH8" s="45"/>
-      <c r="AI8" s="46"/>
-      <c r="AJ8" s="41">
+      <c r="AH8" s="128"/>
+      <c r="AI8" s="131"/>
+      <c r="AJ8" s="124">
         <f>(t_data!$L$9)</f>
         <v>46614</v>
       </c>
-      <c r="AK8" s="42"/>
-      <c r="AL8" s="42"/>
-      <c r="AM8" s="42"/>
-      <c r="AN8" s="42"/>
-      <c r="AO8" s="45">
+      <c r="AK8" s="125"/>
+      <c r="AL8" s="125"/>
+      <c r="AM8" s="125"/>
+      <c r="AN8" s="125"/>
+      <c r="AO8" s="128">
         <f>(t_data!$M$9)</f>
         <v>1487</v>
       </c>
-      <c r="AP8" s="45"/>
-      <c r="AQ8" s="46"/>
-      <c r="AR8" s="41">
+      <c r="AP8" s="128"/>
+      <c r="AQ8" s="131"/>
+      <c r="AR8" s="124">
         <f>(t_data!$L$10)</f>
         <v>47312</v>
       </c>
-      <c r="AS8" s="42"/>
-      <c r="AT8" s="42"/>
-      <c r="AU8" s="42"/>
-      <c r="AV8" s="42"/>
-      <c r="AW8" s="45">
+      <c r="AS8" s="125"/>
+      <c r="AT8" s="125"/>
+      <c r="AU8" s="125"/>
+      <c r="AV8" s="125"/>
+      <c r="AW8" s="128">
         <f>(t_data!$M$10)</f>
         <v>698</v>
       </c>
-      <c r="AX8" s="45"/>
-      <c r="AY8" s="45"/>
-      <c r="AZ8" s="53">
+      <c r="AX8" s="128"/>
+      <c r="AY8" s="128"/>
+      <c r="AZ8" s="144">
         <f>(t_data!M11)</f>
         <v>4701</v>
       </c>
-      <c r="BA8" s="54"/>
-      <c r="BB8" s="54"/>
-      <c r="BC8" s="54"/>
-      <c r="BD8" s="54"/>
-      <c r="BE8" s="54"/>
-      <c r="BF8" s="55"/>
+      <c r="BA8" s="145"/>
+      <c r="BB8" s="145"/>
+      <c r="BC8" s="145"/>
+      <c r="BD8" s="145"/>
+      <c r="BE8" s="145"/>
+      <c r="BF8" s="146"/>
     </row>
     <row r="9" spans="1:58" ht="18.75" customHeight="1">
-      <c r="A9" s="105"/>
-      <c r="B9" s="105"/>
-      <c r="C9" s="105"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="47">
+      <c r="A9" s="137"/>
+      <c r="B9" s="137"/>
+      <c r="C9" s="137"/>
+      <c r="D9" s="126"/>
+      <c r="E9" s="127"/>
+      <c r="F9" s="127"/>
+      <c r="G9" s="127"/>
+      <c r="H9" s="127"/>
+      <c r="I9" s="129">
         <f>(t_data!$N$5)</f>
         <v>3.1693380465837029E-2</v>
       </c>
-      <c r="J9" s="47"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="44"/>
-      <c r="O9" s="44"/>
-      <c r="P9" s="44"/>
-      <c r="Q9" s="47">
+      <c r="J9" s="129"/>
+      <c r="K9" s="132"/>
+      <c r="L9" s="126"/>
+      <c r="M9" s="127"/>
+      <c r="N9" s="127"/>
+      <c r="O9" s="127"/>
+      <c r="P9" s="127"/>
+      <c r="Q9" s="129">
         <f>(t_data!$N$6)</f>
         <v>1.5488958250217122E-2</v>
       </c>
-      <c r="R9" s="47"/>
-      <c r="S9" s="48"/>
-      <c r="T9" s="43"/>
-      <c r="U9" s="44"/>
-      <c r="V9" s="44"/>
-      <c r="W9" s="44"/>
-      <c r="X9" s="44"/>
-      <c r="Y9" s="47">
+      <c r="R9" s="129"/>
+      <c r="S9" s="132"/>
+      <c r="T9" s="126"/>
+      <c r="U9" s="127"/>
+      <c r="V9" s="127"/>
+      <c r="W9" s="127"/>
+      <c r="X9" s="127"/>
+      <c r="Y9" s="129">
         <f>(t_data!$N$7)</f>
         <v>1.2525710059855255E-2</v>
       </c>
-      <c r="Z9" s="47"/>
-      <c r="AA9" s="48"/>
-      <c r="AB9" s="43"/>
-      <c r="AC9" s="44"/>
-      <c r="AD9" s="44"/>
-      <c r="AE9" s="44"/>
-      <c r="AF9" s="44"/>
-      <c r="AG9" s="47">
+      <c r="Z9" s="129"/>
+      <c r="AA9" s="132"/>
+      <c r="AB9" s="126"/>
+      <c r="AC9" s="127"/>
+      <c r="AD9" s="127"/>
+      <c r="AE9" s="127"/>
+      <c r="AF9" s="127"/>
+      <c r="AG9" s="129">
         <f>(t_data!$N$8)</f>
         <v>2.9991098532399008E-2</v>
       </c>
-      <c r="AH9" s="47"/>
-      <c r="AI9" s="48"/>
-      <c r="AJ9" s="43"/>
-      <c r="AK9" s="44"/>
-      <c r="AL9" s="44"/>
-      <c r="AM9" s="44"/>
-      <c r="AN9" s="44"/>
-      <c r="AO9" s="47">
+      <c r="AH9" s="129"/>
+      <c r="AI9" s="132"/>
+      <c r="AJ9" s="126"/>
+      <c r="AK9" s="127"/>
+      <c r="AL9" s="127"/>
+      <c r="AM9" s="127"/>
+      <c r="AN9" s="127"/>
+      <c r="AO9" s="129">
         <f>(t_data!$N$9)</f>
         <v>3.2951448135262629E-2</v>
       </c>
-      <c r="AP9" s="47"/>
-      <c r="AQ9" s="48"/>
-      <c r="AR9" s="43"/>
-      <c r="AS9" s="44"/>
-      <c r="AT9" s="44"/>
-      <c r="AU9" s="44"/>
-      <c r="AV9" s="44"/>
-      <c r="AW9" s="47">
+      <c r="AP9" s="129"/>
+      <c r="AQ9" s="132"/>
+      <c r="AR9" s="126"/>
+      <c r="AS9" s="127"/>
+      <c r="AT9" s="127"/>
+      <c r="AU9" s="127"/>
+      <c r="AV9" s="127"/>
+      <c r="AW9" s="129">
         <f>(t_data!$N$10)</f>
         <v>1.4974042133264698E-2</v>
       </c>
-      <c r="AX9" s="47"/>
-      <c r="AY9" s="47"/>
-      <c r="AZ9" s="56">
+      <c r="AX9" s="129"/>
+      <c r="AY9" s="129"/>
+      <c r="AZ9" s="147">
         <f>(t_data!N11)</f>
         <v>0.11032362535495532</v>
       </c>
-      <c r="BA9" s="57"/>
-      <c r="BB9" s="57"/>
-      <c r="BC9" s="57"/>
-      <c r="BD9" s="57"/>
-      <c r="BE9" s="57"/>
-      <c r="BF9" s="58"/>
+      <c r="BA9" s="148"/>
+      <c r="BB9" s="148"/>
+      <c r="BC9" s="148"/>
+      <c r="BD9" s="148"/>
+      <c r="BE9" s="148"/>
+      <c r="BF9" s="149"/>
     </row>
     <row r="10" spans="1:58" ht="7.5" customHeight="1">
       <c r="A10" s="27"/>
@@ -18304,8 +18303,8 @@
       <c r="AX10" s="27"/>
       <c r="AY10" s="27"/>
       <c r="AZ10" s="27"/>
-      <c r="BA10" s="59"/>
-      <c r="BB10" s="59"/>
+      <c r="BA10" s="150"/>
+      <c r="BB10" s="150"/>
       <c r="BC10" s="27"/>
       <c r="BD10" s="27"/>
       <c r="BE10" s="27"/>
@@ -18373,23 +18372,23 @@
     </row>
     <row r="12" spans="1:58">
       <c r="A12" s="30"/>
-      <c r="B12" s="175" t="s">
+      <c r="B12" s="37" t="s">
         <v>225</v>
       </c>
-      <c r="C12" s="175"/>
-      <c r="D12" s="175"/>
-      <c r="E12" s="175"/>
-      <c r="F12" s="175"/>
-      <c r="G12" s="175"/>
-      <c r="H12" s="175"/>
-      <c r="I12" s="175"/>
-      <c r="J12" s="175"/>
-      <c r="K12" s="175"/>
-      <c r="L12" s="175"/>
-      <c r="M12" s="175"/>
-      <c r="N12" s="175"/>
-      <c r="O12" s="175"/>
-      <c r="P12" s="175"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
       <c r="Q12" s="30"/>
       <c r="R12" s="30"/>
       <c r="S12" s="30"/>
@@ -18399,44 +18398,44 @@
       <c r="W12" s="31"/>
       <c r="X12" s="30"/>
       <c r="Y12" s="30"/>
-      <c r="Z12" s="174" t="str">
+      <c r="Z12" s="60" t="str">
         <f>(g_data!B43)</f>
         <v>2020-08-01</v>
       </c>
-      <c r="AA12" s="174"/>
-      <c r="AB12" s="174"/>
-      <c r="AC12" s="174"/>
-      <c r="AD12" s="174"/>
-      <c r="AE12" s="174"/>
-      <c r="AF12" s="174"/>
-      <c r="AG12" s="174"/>
-      <c r="AH12" s="174"/>
-      <c r="AI12" s="174"/>
-      <c r="AJ12" s="174"/>
-      <c r="AK12" s="174"/>
-      <c r="AL12" s="174"/>
-      <c r="AM12" s="174"/>
-      <c r="AN12" s="174"/>
+      <c r="AA12" s="60"/>
+      <c r="AB12" s="60"/>
+      <c r="AC12" s="60"/>
+      <c r="AD12" s="60"/>
+      <c r="AE12" s="60"/>
+      <c r="AF12" s="60"/>
+      <c r="AG12" s="60"/>
+      <c r="AH12" s="60"/>
+      <c r="AI12" s="60"/>
+      <c r="AJ12" s="60"/>
+      <c r="AK12" s="60"/>
+      <c r="AL12" s="60"/>
+      <c r="AM12" s="60"/>
+      <c r="AN12" s="60"/>
       <c r="AO12" s="30"/>
       <c r="AP12" s="30"/>
-      <c r="AQ12" s="174" t="str">
+      <c r="AQ12" s="60" t="str">
         <f>(g_data!B48)</f>
         <v>2025-08-01</v>
       </c>
-      <c r="AR12" s="174"/>
-      <c r="AS12" s="174"/>
-      <c r="AT12" s="174"/>
-      <c r="AU12" s="174"/>
-      <c r="AV12" s="174"/>
-      <c r="AW12" s="174"/>
-      <c r="AX12" s="174"/>
-      <c r="AY12" s="174"/>
-      <c r="AZ12" s="174"/>
-      <c r="BA12" s="174"/>
-      <c r="BB12" s="174"/>
-      <c r="BC12" s="174"/>
-      <c r="BD12" s="174"/>
-      <c r="BE12" s="174"/>
+      <c r="AR12" s="60"/>
+      <c r="AS12" s="60"/>
+      <c r="AT12" s="60"/>
+      <c r="AU12" s="60"/>
+      <c r="AV12" s="60"/>
+      <c r="AW12" s="60"/>
+      <c r="AX12" s="60"/>
+      <c r="AY12" s="60"/>
+      <c r="AZ12" s="60"/>
+      <c r="BA12" s="60"/>
+      <c r="BB12" s="60"/>
+      <c r="BC12" s="60"/>
+      <c r="BD12" s="60"/>
+      <c r="BE12" s="60"/>
       <c r="BF12" s="27"/>
     </row>
     <row r="13" spans="1:58">
@@ -19280,59 +19279,59 @@
       <c r="BF26" s="27"/>
     </row>
     <row r="27" spans="1:58">
-      <c r="A27" s="136" t="s">
+      <c r="A27" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="136"/>
-      <c r="C27" s="136"/>
-      <c r="D27" s="136"/>
-      <c r="E27" s="136"/>
-      <c r="F27" s="136"/>
-      <c r="G27" s="136"/>
-      <c r="H27" s="136"/>
-      <c r="I27" s="136"/>
-      <c r="J27" s="136"/>
-      <c r="K27" s="136"/>
-      <c r="L27" s="136"/>
-      <c r="M27" s="136"/>
-      <c r="N27" s="136"/>
-      <c r="O27" s="136"/>
-      <c r="P27" s="136"/>
-      <c r="Q27" s="136"/>
-      <c r="R27" s="136"/>
-      <c r="S27" s="136"/>
-      <c r="T27" s="136"/>
-      <c r="U27" s="136"/>
-      <c r="V27" s="136"/>
-      <c r="W27" s="136"/>
-      <c r="X27" s="136"/>
-      <c r="Y27" s="136"/>
-      <c r="Z27" s="136"/>
-      <c r="AA27" s="136"/>
-      <c r="AB27" s="136"/>
-      <c r="AC27" s="136"/>
-      <c r="AD27" s="136"/>
-      <c r="AE27" s="136"/>
-      <c r="AF27" s="136"/>
-      <c r="AG27" s="136"/>
-      <c r="AH27" s="136"/>
-      <c r="AI27" s="136"/>
-      <c r="AJ27" s="136"/>
-      <c r="AK27" s="136"/>
-      <c r="AL27" s="136"/>
-      <c r="AM27" s="136"/>
-      <c r="AN27" s="136"/>
-      <c r="AO27" s="136"/>
-      <c r="AP27" s="136"/>
-      <c r="AQ27" s="136"/>
-      <c r="AR27" s="136"/>
-      <c r="AS27" s="136"/>
-      <c r="AT27" s="136"/>
-      <c r="AU27" s="136"/>
-      <c r="AV27" s="136"/>
-      <c r="AW27" s="136"/>
-      <c r="AX27" s="136"/>
-      <c r="AY27" s="136"/>
+      <c r="B27" s="96"/>
+      <c r="C27" s="96"/>
+      <c r="D27" s="96"/>
+      <c r="E27" s="96"/>
+      <c r="F27" s="96"/>
+      <c r="G27" s="96"/>
+      <c r="H27" s="96"/>
+      <c r="I27" s="96"/>
+      <c r="J27" s="96"/>
+      <c r="K27" s="96"/>
+      <c r="L27" s="96"/>
+      <c r="M27" s="96"/>
+      <c r="N27" s="96"/>
+      <c r="O27" s="96"/>
+      <c r="P27" s="96"/>
+      <c r="Q27" s="96"/>
+      <c r="R27" s="96"/>
+      <c r="S27" s="96"/>
+      <c r="T27" s="96"/>
+      <c r="U27" s="96"/>
+      <c r="V27" s="96"/>
+      <c r="W27" s="96"/>
+      <c r="X27" s="96"/>
+      <c r="Y27" s="96"/>
+      <c r="Z27" s="96"/>
+      <c r="AA27" s="96"/>
+      <c r="AB27" s="96"/>
+      <c r="AC27" s="96"/>
+      <c r="AD27" s="96"/>
+      <c r="AE27" s="96"/>
+      <c r="AF27" s="96"/>
+      <c r="AG27" s="96"/>
+      <c r="AH27" s="96"/>
+      <c r="AI27" s="96"/>
+      <c r="AJ27" s="96"/>
+      <c r="AK27" s="96"/>
+      <c r="AL27" s="96"/>
+      <c r="AM27" s="96"/>
+      <c r="AN27" s="96"/>
+      <c r="AO27" s="96"/>
+      <c r="AP27" s="96"/>
+      <c r="AQ27" s="96"/>
+      <c r="AR27" s="96"/>
+      <c r="AS27" s="96"/>
+      <c r="AT27" s="96"/>
+      <c r="AU27" s="96"/>
+      <c r="AV27" s="96"/>
+      <c r="AW27" s="96"/>
+      <c r="AX27" s="96"/>
+      <c r="AY27" s="96"/>
       <c r="AZ27" s="27"/>
       <c r="BA27" s="27"/>
       <c r="BB27" s="27"/>
@@ -19342,684 +19341,684 @@
       <c r="BF27" s="27"/>
     </row>
     <row r="28" spans="1:58">
-      <c r="A28" s="125"/>
-      <c r="B28" s="125"/>
-      <c r="C28" s="125"/>
-      <c r="D28" s="124" t="str">
+      <c r="A28" s="49"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="48" t="str">
         <f>(t_data!$B$5)</f>
         <v>2020-08-01</v>
       </c>
-      <c r="E28" s="125"/>
-      <c r="F28" s="125"/>
-      <c r="G28" s="125"/>
-      <c r="H28" s="125"/>
-      <c r="I28" s="125"/>
-      <c r="J28" s="125"/>
-      <c r="K28" s="125"/>
-      <c r="L28" s="124" t="str">
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="48" t="str">
         <f>(t_data!$B$6)</f>
         <v>2021-08-01</v>
       </c>
-      <c r="M28" s="125"/>
-      <c r="N28" s="125"/>
-      <c r="O28" s="125"/>
-      <c r="P28" s="125"/>
-      <c r="Q28" s="125"/>
-      <c r="R28" s="125"/>
-      <c r="S28" s="125"/>
-      <c r="T28" s="124" t="str">
+      <c r="M28" s="49"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="49"/>
+      <c r="P28" s="49"/>
+      <c r="Q28" s="49"/>
+      <c r="R28" s="49"/>
+      <c r="S28" s="49"/>
+      <c r="T28" s="48" t="str">
         <f>(t_data!$B$7)</f>
         <v>2022-08-01</v>
       </c>
-      <c r="U28" s="125"/>
-      <c r="V28" s="125"/>
-      <c r="W28" s="125"/>
-      <c r="X28" s="125"/>
-      <c r="Y28" s="125"/>
-      <c r="Z28" s="125"/>
-      <c r="AA28" s="125"/>
-      <c r="AB28" s="124" t="str">
+      <c r="U28" s="49"/>
+      <c r="V28" s="49"/>
+      <c r="W28" s="49"/>
+      <c r="X28" s="49"/>
+      <c r="Y28" s="49"/>
+      <c r="Z28" s="49"/>
+      <c r="AA28" s="49"/>
+      <c r="AB28" s="48" t="str">
         <f>(t_data!$B$8)</f>
         <v>2023-08-01</v>
       </c>
-      <c r="AC28" s="125"/>
-      <c r="AD28" s="125"/>
-      <c r="AE28" s="125"/>
-      <c r="AF28" s="125"/>
-      <c r="AG28" s="125"/>
-      <c r="AH28" s="125"/>
-      <c r="AI28" s="125"/>
-      <c r="AJ28" s="124" t="str">
+      <c r="AC28" s="49"/>
+      <c r="AD28" s="49"/>
+      <c r="AE28" s="49"/>
+      <c r="AF28" s="49"/>
+      <c r="AG28" s="49"/>
+      <c r="AH28" s="49"/>
+      <c r="AI28" s="49"/>
+      <c r="AJ28" s="48" t="str">
         <f>(t_data!$B$9)</f>
         <v>2024-08-01</v>
       </c>
-      <c r="AK28" s="125"/>
-      <c r="AL28" s="125"/>
-      <c r="AM28" s="125"/>
-      <c r="AN28" s="125"/>
-      <c r="AO28" s="125"/>
-      <c r="AP28" s="125"/>
-      <c r="AQ28" s="125"/>
-      <c r="AR28" s="124" t="str">
+      <c r="AK28" s="49"/>
+      <c r="AL28" s="49"/>
+      <c r="AM28" s="49"/>
+      <c r="AN28" s="49"/>
+      <c r="AO28" s="49"/>
+      <c r="AP28" s="49"/>
+      <c r="AQ28" s="49"/>
+      <c r="AR28" s="48" t="str">
         <f>(t_data!$B$10)</f>
         <v>2025-08-01</v>
       </c>
-      <c r="AS28" s="125"/>
-      <c r="AT28" s="125"/>
-      <c r="AU28" s="125"/>
-      <c r="AV28" s="125"/>
-      <c r="AW28" s="125"/>
-      <c r="AX28" s="125"/>
-      <c r="AY28" s="126"/>
-      <c r="AZ28" s="97" t="s">
-        <v>228</v>
-      </c>
-      <c r="BA28" s="95"/>
-      <c r="BB28" s="95"/>
-      <c r="BC28" s="95"/>
-      <c r="BD28" s="95"/>
-      <c r="BE28" s="95"/>
-      <c r="BF28" s="96"/>
+      <c r="AS28" s="49"/>
+      <c r="AT28" s="49"/>
+      <c r="AU28" s="49"/>
+      <c r="AV28" s="49"/>
+      <c r="AW28" s="49"/>
+      <c r="AX28" s="49"/>
+      <c r="AY28" s="50"/>
+      <c r="AZ28" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="BA28" s="134"/>
+      <c r="BB28" s="134"/>
+      <c r="BC28" s="134"/>
+      <c r="BD28" s="134"/>
+      <c r="BE28" s="134"/>
+      <c r="BF28" s="135"/>
     </row>
     <row r="29" spans="1:58">
-      <c r="A29" s="133" t="s">
+      <c r="A29" s="106" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="133"/>
-      <c r="C29" s="133"/>
-      <c r="D29" s="127">
+      <c r="B29" s="106"/>
+      <c r="C29" s="106"/>
+      <c r="D29" s="83">
         <f>(t_data!$U$5)</f>
         <v>15285</v>
       </c>
-      <c r="E29" s="128"/>
-      <c r="F29" s="128"/>
-      <c r="G29" s="128"/>
-      <c r="H29" s="134">
+      <c r="E29" s="84"/>
+      <c r="F29" s="84"/>
+      <c r="G29" s="84"/>
+      <c r="H29" s="61">
         <f>(D29/D5)</f>
         <v>0.19281956831628211</v>
       </c>
-      <c r="I29" s="134"/>
-      <c r="J29" s="131">
+      <c r="I29" s="61"/>
+      <c r="J29" s="63">
         <f>(t_data!$V$5)</f>
         <v>129</v>
       </c>
-      <c r="K29" s="132"/>
-      <c r="L29" s="127">
+      <c r="K29" s="82"/>
+      <c r="L29" s="83">
         <f>(t_data!$U$6)</f>
         <v>15140</v>
       </c>
-      <c r="M29" s="128"/>
-      <c r="N29" s="128"/>
-      <c r="O29" s="128"/>
-      <c r="P29" s="134">
+      <c r="M29" s="84"/>
+      <c r="N29" s="84"/>
+      <c r="O29" s="84"/>
+      <c r="P29" s="61">
         <f>(L29/L5)</f>
         <v>0.18951532145003006</v>
       </c>
-      <c r="Q29" s="134"/>
-      <c r="R29" s="131">
+      <c r="Q29" s="61"/>
+      <c r="R29" s="63">
         <f>(t_data!$V$6)</f>
         <v>-145</v>
       </c>
-      <c r="S29" s="132"/>
-      <c r="T29" s="127">
+      <c r="S29" s="82"/>
+      <c r="T29" s="83">
         <f>(t_data!$U$7)</f>
         <v>15145</v>
       </c>
-      <c r="U29" s="128"/>
-      <c r="V29" s="128"/>
-      <c r="W29" s="128"/>
-      <c r="X29" s="134">
+      <c r="U29" s="84"/>
+      <c r="V29" s="84"/>
+      <c r="W29" s="84"/>
+      <c r="X29" s="61">
         <f>(T29/T5)</f>
         <v>0.18899357334498035</v>
       </c>
-      <c r="Y29" s="134"/>
-      <c r="Z29" s="131">
+      <c r="Y29" s="61"/>
+      <c r="Z29" s="63">
         <f>(t_data!$V$7)</f>
         <v>5</v>
       </c>
-      <c r="AA29" s="132"/>
-      <c r="AB29" s="127">
+      <c r="AA29" s="82"/>
+      <c r="AB29" s="83">
         <f>(t_data!$U$8)</f>
         <v>15063</v>
       </c>
-      <c r="AC29" s="128"/>
-      <c r="AD29" s="128"/>
-      <c r="AE29" s="128"/>
-      <c r="AF29" s="134">
+      <c r="AC29" s="84"/>
+      <c r="AD29" s="84"/>
+      <c r="AE29" s="84"/>
+      <c r="AF29" s="61">
         <f>(AB29/AB5)</f>
         <v>0.18441930507603027</v>
       </c>
-      <c r="AG29" s="134"/>
-      <c r="AH29" s="131">
+      <c r="AG29" s="61"/>
+      <c r="AH29" s="63">
         <f>(t_data!$V$8)</f>
         <v>-82</v>
       </c>
-      <c r="AI29" s="132"/>
-      <c r="AJ29" s="127">
+      <c r="AI29" s="82"/>
+      <c r="AJ29" s="83">
         <f>(t_data!$U$9)</f>
         <v>15112</v>
       </c>
-      <c r="AK29" s="128"/>
-      <c r="AL29" s="128"/>
-      <c r="AM29" s="128"/>
-      <c r="AN29" s="134">
+      <c r="AK29" s="84"/>
+      <c r="AL29" s="84"/>
+      <c r="AM29" s="84"/>
+      <c r="AN29" s="61">
         <f>(AJ29/AJ5)</f>
         <v>0.18151026340127557</v>
       </c>
-      <c r="AO29" s="134"/>
-      <c r="AP29" s="131">
+      <c r="AO29" s="61"/>
+      <c r="AP29" s="63">
         <f>(t_data!$V$9)</f>
         <v>49</v>
       </c>
-      <c r="AQ29" s="132"/>
-      <c r="AR29" s="127">
+      <c r="AQ29" s="82"/>
+      <c r="AR29" s="83">
         <f>(t_data!$U$10)</f>
         <v>15185</v>
       </c>
-      <c r="AS29" s="128"/>
-      <c r="AT29" s="128"/>
-      <c r="AU29" s="128"/>
-      <c r="AV29" s="134">
+      <c r="AS29" s="84"/>
+      <c r="AT29" s="84"/>
+      <c r="AU29" s="84"/>
+      <c r="AV29" s="61">
         <f>(AR29/AR5)</f>
         <v>0.18135674190851547</v>
       </c>
-      <c r="AW29" s="134"/>
-      <c r="AX29" s="131">
+      <c r="AW29" s="61"/>
+      <c r="AX29" s="63">
         <f>(t_data!$V$10)</f>
         <v>73</v>
       </c>
-      <c r="AY29" s="131"/>
-      <c r="AZ29" s="76">
+      <c r="AY29" s="63"/>
+      <c r="AZ29" s="164">
         <f>(t_data!V11)</f>
         <v>-100</v>
       </c>
-      <c r="BA29" s="77"/>
-      <c r="BB29" s="77"/>
-      <c r="BC29" s="77"/>
-      <c r="BD29" s="77"/>
-      <c r="BE29" s="77"/>
-      <c r="BF29" s="78"/>
+      <c r="BA29" s="165"/>
+      <c r="BB29" s="165"/>
+      <c r="BC29" s="165"/>
+      <c r="BD29" s="165"/>
+      <c r="BE29" s="165"/>
+      <c r="BF29" s="166"/>
     </row>
     <row r="30" spans="1:58">
-      <c r="A30" s="133"/>
-      <c r="B30" s="133"/>
-      <c r="C30" s="133"/>
-      <c r="D30" s="129"/>
-      <c r="E30" s="130"/>
-      <c r="F30" s="130"/>
-      <c r="G30" s="130"/>
-      <c r="H30" s="135"/>
-      <c r="I30" s="135"/>
-      <c r="J30" s="171">
+      <c r="A30" s="106"/>
+      <c r="B30" s="106"/>
+      <c r="C30" s="106"/>
+      <c r="D30" s="85"/>
+      <c r="E30" s="86"/>
+      <c r="F30" s="86"/>
+      <c r="G30" s="86"/>
+      <c r="H30" s="62"/>
+      <c r="I30" s="62"/>
+      <c r="J30" s="57">
         <f>(t_data!$W$5)</f>
         <v>8.5114806017418942E-3</v>
       </c>
-      <c r="K30" s="172"/>
-      <c r="L30" s="129"/>
-      <c r="M30" s="130"/>
-      <c r="N30" s="130"/>
-      <c r="O30" s="130"/>
-      <c r="P30" s="135"/>
-      <c r="Q30" s="135"/>
-      <c r="R30" s="171">
+      <c r="K30" s="58"/>
+      <c r="L30" s="85"/>
+      <c r="M30" s="86"/>
+      <c r="N30" s="86"/>
+      <c r="O30" s="86"/>
+      <c r="P30" s="62"/>
+      <c r="Q30" s="62"/>
+      <c r="R30" s="57">
         <f>(t_data!$W$6)</f>
         <v>-9.4864245992802854E-3</v>
       </c>
-      <c r="S30" s="172"/>
-      <c r="T30" s="129"/>
-      <c r="U30" s="130"/>
-      <c r="V30" s="130"/>
-      <c r="W30" s="130"/>
-      <c r="X30" s="135"/>
-      <c r="Y30" s="135"/>
-      <c r="Z30" s="171">
+      <c r="S30" s="58"/>
+      <c r="T30" s="85"/>
+      <c r="U30" s="86"/>
+      <c r="V30" s="86"/>
+      <c r="W30" s="86"/>
+      <c r="X30" s="62"/>
+      <c r="Y30" s="62"/>
+      <c r="Z30" s="57">
         <f>(t_data!$W$7)</f>
         <v>3.3025099075301156E-4</v>
       </c>
-      <c r="AA30" s="172"/>
-      <c r="AB30" s="129"/>
-      <c r="AC30" s="130"/>
-      <c r="AD30" s="130"/>
-      <c r="AE30" s="130"/>
-      <c r="AF30" s="135"/>
-      <c r="AG30" s="135"/>
-      <c r="AH30" s="171">
+      <c r="AA30" s="58"/>
+      <c r="AB30" s="85"/>
+      <c r="AC30" s="86"/>
+      <c r="AD30" s="86"/>
+      <c r="AE30" s="86"/>
+      <c r="AF30" s="62"/>
+      <c r="AG30" s="62"/>
+      <c r="AH30" s="57">
         <f>(t_data!$W$8)</f>
         <v>-5.4143281611093164E-3</v>
       </c>
-      <c r="AI30" s="172"/>
-      <c r="AJ30" s="129"/>
-      <c r="AK30" s="130"/>
-      <c r="AL30" s="130"/>
-      <c r="AM30" s="130"/>
-      <c r="AN30" s="135"/>
-      <c r="AO30" s="135"/>
-      <c r="AP30" s="171">
+      <c r="AI30" s="58"/>
+      <c r="AJ30" s="85"/>
+      <c r="AK30" s="86"/>
+      <c r="AL30" s="86"/>
+      <c r="AM30" s="86"/>
+      <c r="AN30" s="62"/>
+      <c r="AO30" s="62"/>
+      <c r="AP30" s="57">
         <f>(t_data!$W$9)</f>
         <v>3.2530040496581147E-3</v>
       </c>
-      <c r="AQ30" s="172"/>
-      <c r="AR30" s="129"/>
-      <c r="AS30" s="130"/>
-      <c r="AT30" s="130"/>
-      <c r="AU30" s="130"/>
-      <c r="AV30" s="135"/>
-      <c r="AW30" s="135"/>
-      <c r="AX30" s="171">
+      <c r="AQ30" s="58"/>
+      <c r="AR30" s="85"/>
+      <c r="AS30" s="86"/>
+      <c r="AT30" s="86"/>
+      <c r="AU30" s="86"/>
+      <c r="AV30" s="62"/>
+      <c r="AW30" s="62"/>
+      <c r="AX30" s="57">
         <f>(t_data!$W$10)</f>
         <v>4.8305982001057846E-3</v>
       </c>
-      <c r="AY30" s="171"/>
-      <c r="AZ30" s="79">
+      <c r="AY30" s="57"/>
+      <c r="AZ30" s="167">
         <f>(t_data!W11)</f>
         <v>-6.5423617926071431E-3</v>
       </c>
-      <c r="BA30" s="80"/>
-      <c r="BB30" s="80"/>
-      <c r="BC30" s="80"/>
-      <c r="BD30" s="80"/>
-      <c r="BE30" s="80"/>
-      <c r="BF30" s="81"/>
+      <c r="BA30" s="168"/>
+      <c r="BB30" s="168"/>
+      <c r="BC30" s="168"/>
+      <c r="BD30" s="168"/>
+      <c r="BE30" s="168"/>
+      <c r="BF30" s="169"/>
     </row>
     <row r="31" spans="1:58">
-      <c r="A31" s="137" t="s">
+      <c r="A31" s="107" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="137"/>
-      <c r="C31" s="137"/>
-      <c r="D31" s="138">
+      <c r="B31" s="107"/>
+      <c r="C31" s="107"/>
+      <c r="D31" s="68">
         <f>(t_data!$R$5)</f>
         <v>54447</v>
       </c>
-      <c r="E31" s="139"/>
-      <c r="F31" s="139"/>
-      <c r="G31" s="139"/>
-      <c r="H31" s="115">
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="72">
         <f>(D31/D5)</f>
         <v>0.686846387707989</v>
       </c>
-      <c r="I31" s="115"/>
-      <c r="J31" s="142">
+      <c r="I31" s="72"/>
+      <c r="J31" s="66">
         <f>(t_data!$S$5)</f>
         <v>1601</v>
       </c>
-      <c r="K31" s="143"/>
-      <c r="L31" s="138">
+      <c r="K31" s="67"/>
+      <c r="L31" s="68">
         <f>(t_data!$R$6)</f>
         <v>55075</v>
       </c>
-      <c r="M31" s="139"/>
-      <c r="N31" s="139"/>
-      <c r="O31" s="139"/>
-      <c r="P31" s="115">
+      <c r="M31" s="69"/>
+      <c r="N31" s="69"/>
+      <c r="O31" s="69"/>
+      <c r="P31" s="72">
         <f>(L31/L5)</f>
         <v>0.68940266372922088</v>
       </c>
-      <c r="Q31" s="115"/>
-      <c r="R31" s="142">
+      <c r="Q31" s="72"/>
+      <c r="R31" s="66">
         <f>(t_data!$S$6)</f>
         <v>628</v>
       </c>
-      <c r="S31" s="143"/>
-      <c r="T31" s="138">
-        <f>(t_data!$R$6)</f>
-        <v>55075</v>
-      </c>
-      <c r="U31" s="139"/>
-      <c r="V31" s="139"/>
-      <c r="W31" s="139"/>
-      <c r="X31" s="115">
+      <c r="S31" s="67"/>
+      <c r="T31" s="68">
+        <f>(t_data!$R$7)</f>
+        <v>55435</v>
+      </c>
+      <c r="U31" s="69"/>
+      <c r="V31" s="69"/>
+      <c r="W31" s="69"/>
+      <c r="X31" s="72">
         <f>(T31/T5)</f>
-        <v>0.68727771884944155</v>
-      </c>
-      <c r="Y31" s="115"/>
-      <c r="Z31" s="142">
-        <f>(t_data!$S$6)</f>
-        <v>628</v>
-      </c>
-      <c r="AA31" s="143"/>
-      <c r="AB31" s="138">
-        <f>(t_data!$R$6)</f>
-        <v>55075</v>
-      </c>
-      <c r="AC31" s="139"/>
-      <c r="AD31" s="139"/>
-      <c r="AE31" s="139"/>
-      <c r="AF31" s="115">
+        <v>0.69177013789230668</v>
+      </c>
+      <c r="Y31" s="72"/>
+      <c r="Z31" s="66">
+        <f>(t_data!$S$7)</f>
+        <v>360</v>
+      </c>
+      <c r="AA31" s="67"/>
+      <c r="AB31" s="68">
+        <f>(t_data!$R$8)</f>
+        <v>56958</v>
+      </c>
+      <c r="AC31" s="69"/>
+      <c r="AD31" s="69"/>
+      <c r="AE31" s="69"/>
+      <c r="AF31" s="72">
         <f>(AB31/AB5)</f>
-        <v>0.67429417958324156</v>
-      </c>
-      <c r="AG31" s="115"/>
-      <c r="AH31" s="142">
-        <f>(t_data!$S$6)</f>
-        <v>628</v>
-      </c>
-      <c r="AI31" s="143"/>
-      <c r="AJ31" s="138">
-        <f>(t_data!$R$6)</f>
-        <v>55075</v>
-      </c>
-      <c r="AK31" s="139"/>
-      <c r="AL31" s="139"/>
-      <c r="AM31" s="139"/>
-      <c r="AN31" s="115">
+        <v>0.69734812311760819</v>
+      </c>
+      <c r="AG31" s="72"/>
+      <c r="AH31" s="66">
+        <f>(t_data!$S$8)</f>
+        <v>1523</v>
+      </c>
+      <c r="AI31" s="67"/>
+      <c r="AJ31" s="68">
+        <f>(t_data!$R$9)</f>
+        <v>58548</v>
+      </c>
+      <c r="AK31" s="69"/>
+      <c r="AL31" s="69"/>
+      <c r="AM31" s="69"/>
+      <c r="AN31" s="72">
         <f>(AJ31/AJ5)</f>
-        <v>0.66150593944052749</v>
-      </c>
-      <c r="AO31" s="115"/>
-      <c r="AP31" s="142">
-        <f>(t_data!$S$6)</f>
-        <v>628</v>
-      </c>
-      <c r="AQ31" s="143"/>
-      <c r="AR31" s="138">
-        <f>(t_data!$R$6)</f>
-        <v>55075</v>
-      </c>
-      <c r="AS31" s="139"/>
-      <c r="AT31" s="139"/>
-      <c r="AU31" s="139"/>
-      <c r="AV31" s="115">
+        <v>0.7032201496570859</v>
+      </c>
+      <c r="AO31" s="72"/>
+      <c r="AP31" s="66">
+        <f>(t_data!$S$9)</f>
+        <v>1590</v>
+      </c>
+      <c r="AQ31" s="67"/>
+      <c r="AR31" s="68">
+        <f>(t_data!$R$10)</f>
+        <v>59115</v>
+      </c>
+      <c r="AS31" s="69"/>
+      <c r="AT31" s="69"/>
+      <c r="AU31" s="69"/>
+      <c r="AV31" s="72">
         <f>(AR31/AR5)</f>
-        <v>0.65776901946733546</v>
-      </c>
-      <c r="AW31" s="115"/>
-      <c r="AX31" s="142">
-        <f>(t_data!$S$6)</f>
-        <v>628</v>
-      </c>
-      <c r="AY31" s="142"/>
-      <c r="AZ31" s="82">
+        <v>0.70601934790397702</v>
+      </c>
+      <c r="AW31" s="72"/>
+      <c r="AX31" s="66">
+        <f>(t_data!$S$10)</f>
+        <v>567</v>
+      </c>
+      <c r="AY31" s="66"/>
+      <c r="AZ31" s="170">
         <f>(t_data!S11)</f>
         <v>4668</v>
       </c>
-      <c r="BA31" s="83"/>
-      <c r="BB31" s="83"/>
-      <c r="BC31" s="83"/>
-      <c r="BD31" s="83"/>
-      <c r="BE31" s="83"/>
-      <c r="BF31" s="84"/>
+      <c r="BA31" s="171"/>
+      <c r="BB31" s="171"/>
+      <c r="BC31" s="171"/>
+      <c r="BD31" s="171"/>
+      <c r="BE31" s="171"/>
+      <c r="BF31" s="172"/>
     </row>
     <row r="32" spans="1:58">
-      <c r="A32" s="137"/>
-      <c r="B32" s="137"/>
-      <c r="C32" s="137"/>
-      <c r="D32" s="140"/>
-      <c r="E32" s="141"/>
-      <c r="F32" s="141"/>
-      <c r="G32" s="141"/>
-      <c r="H32" s="116"/>
-      <c r="I32" s="116"/>
-      <c r="J32" s="169">
+      <c r="A32" s="107"/>
+      <c r="B32" s="107"/>
+      <c r="C32" s="107"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="73"/>
+      <c r="I32" s="73"/>
+      <c r="J32" s="80">
         <f>(t_data!$T$5)</f>
         <v>3.0295575824092591E-2</v>
       </c>
-      <c r="K32" s="170"/>
-      <c r="L32" s="140"/>
-      <c r="M32" s="141"/>
-      <c r="N32" s="141"/>
-      <c r="O32" s="141"/>
-      <c r="P32" s="116"/>
-      <c r="Q32" s="116"/>
-      <c r="R32" s="169">
+      <c r="K32" s="81"/>
+      <c r="L32" s="70"/>
+      <c r="M32" s="71"/>
+      <c r="N32" s="71"/>
+      <c r="O32" s="71"/>
+      <c r="P32" s="73"/>
+      <c r="Q32" s="73"/>
+      <c r="R32" s="80">
         <f>(t_data!$T$6)</f>
         <v>1.1534152478557047E-2</v>
       </c>
-      <c r="S32" s="170"/>
-      <c r="T32" s="140"/>
-      <c r="U32" s="141"/>
-      <c r="V32" s="141"/>
-      <c r="W32" s="141"/>
-      <c r="X32" s="116"/>
-      <c r="Y32" s="116"/>
-      <c r="Z32" s="169">
-        <f>(t_data!$T$6)</f>
-        <v>1.1534152478557047E-2</v>
-      </c>
-      <c r="AA32" s="170"/>
-      <c r="AB32" s="140"/>
-      <c r="AC32" s="141"/>
-      <c r="AD32" s="141"/>
-      <c r="AE32" s="141"/>
-      <c r="AF32" s="116"/>
-      <c r="AG32" s="116"/>
-      <c r="AH32" s="169">
-        <f>(t_data!$T$6)</f>
-        <v>1.1534152478557047E-2</v>
-      </c>
-      <c r="AI32" s="170"/>
-      <c r="AJ32" s="140"/>
-      <c r="AK32" s="141"/>
-      <c r="AL32" s="141"/>
-      <c r="AM32" s="141"/>
-      <c r="AN32" s="116"/>
-      <c r="AO32" s="116"/>
-      <c r="AP32" s="169">
-        <f>(t_data!$T$6)</f>
-        <v>1.1534152478557047E-2</v>
-      </c>
-      <c r="AQ32" s="170"/>
-      <c r="AR32" s="140"/>
-      <c r="AS32" s="141"/>
-      <c r="AT32" s="141"/>
-      <c r="AU32" s="141"/>
-      <c r="AV32" s="116"/>
-      <c r="AW32" s="116"/>
-      <c r="AX32" s="169">
-        <f>(t_data!$T$6)</f>
-        <v>1.1534152478557047E-2</v>
-      </c>
-      <c r="AY32" s="169"/>
-      <c r="AZ32" s="85">
+      <c r="S32" s="81"/>
+      <c r="T32" s="70"/>
+      <c r="U32" s="71"/>
+      <c r="V32" s="71"/>
+      <c r="W32" s="71"/>
+      <c r="X32" s="73"/>
+      <c r="Y32" s="73"/>
+      <c r="Z32" s="80">
+        <f>(t_data!$T$7)</f>
+        <v>6.5365410803450708E-3</v>
+      </c>
+      <c r="AA32" s="81"/>
+      <c r="AB32" s="70"/>
+      <c r="AC32" s="71"/>
+      <c r="AD32" s="71"/>
+      <c r="AE32" s="71"/>
+      <c r="AF32" s="73"/>
+      <c r="AG32" s="73"/>
+      <c r="AH32" s="80">
+        <f>(t_data!$T$8)</f>
+        <v>2.7473617750518597E-2</v>
+      </c>
+      <c r="AI32" s="81"/>
+      <c r="AJ32" s="70"/>
+      <c r="AK32" s="71"/>
+      <c r="AL32" s="71"/>
+      <c r="AM32" s="71"/>
+      <c r="AN32" s="73"/>
+      <c r="AO32" s="73"/>
+      <c r="AP32" s="80">
+        <f>(t_data!$T$9)</f>
+        <v>2.7915306014958396E-2</v>
+      </c>
+      <c r="AQ32" s="81"/>
+      <c r="AR32" s="70"/>
+      <c r="AS32" s="71"/>
+      <c r="AT32" s="71"/>
+      <c r="AU32" s="71"/>
+      <c r="AV32" s="73"/>
+      <c r="AW32" s="73"/>
+      <c r="AX32" s="80">
+        <f>(t_data!$T$10)</f>
+        <v>9.6843615494979218E-3</v>
+      </c>
+      <c r="AY32" s="80"/>
+      <c r="AZ32" s="173">
         <f>(t_data!T11)</f>
         <v>8.5734751225962968E-2</v>
       </c>
-      <c r="BA32" s="86"/>
-      <c r="BB32" s="86"/>
-      <c r="BC32" s="86"/>
-      <c r="BD32" s="86"/>
-      <c r="BE32" s="86"/>
-      <c r="BF32" s="87"/>
+      <c r="BA32" s="174"/>
+      <c r="BB32" s="174"/>
+      <c r="BC32" s="174"/>
+      <c r="BD32" s="174"/>
+      <c r="BE32" s="174"/>
+      <c r="BF32" s="175"/>
     </row>
     <row r="33" spans="1:58">
-      <c r="A33" s="123" t="s">
+      <c r="A33" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="123"/>
-      <c r="C33" s="123"/>
-      <c r="D33" s="117">
+      <c r="B33" s="105"/>
+      <c r="C33" s="105"/>
+      <c r="D33" s="99">
+        <f>(t_data!$O$5)</f>
+        <v>9540</v>
+      </c>
+      <c r="E33" s="100"/>
+      <c r="F33" s="100"/>
+      <c r="G33" s="100"/>
+      <c r="H33" s="103">
+        <f>(D33/D5)</f>
+        <v>0.12034665892949502</v>
+      </c>
+      <c r="I33" s="103"/>
+      <c r="J33" s="97">
+        <f>(t_data!$P$5)</f>
+        <v>393</v>
+      </c>
+      <c r="K33" s="98"/>
+      <c r="L33" s="99">
         <f>(t_data!$O$6)</f>
         <v>9671</v>
       </c>
-      <c r="E33" s="118"/>
-      <c r="F33" s="118"/>
-      <c r="G33" s="118"/>
-      <c r="H33" s="121">
-        <f>(D33/D5)</f>
-        <v>0.12199921787286649</v>
-      </c>
-      <c r="I33" s="121"/>
-      <c r="J33" s="147">
+      <c r="M33" s="100"/>
+      <c r="N33" s="100"/>
+      <c r="O33" s="100"/>
+      <c r="P33" s="103">
+        <f>(L33/L5)</f>
+        <v>0.12105697977168035</v>
+      </c>
+      <c r="Q33" s="103"/>
+      <c r="R33" s="97">
         <f>(t_data!$P$6)</f>
         <v>131</v>
       </c>
-      <c r="K33" s="148"/>
-      <c r="L33" s="117">
-        <f>(t_data!$O$6)</f>
-        <v>9671</v>
-      </c>
-      <c r="M33" s="118"/>
-      <c r="N33" s="118"/>
-      <c r="O33" s="118"/>
-      <c r="P33" s="121">
-        <f>(L33/L5)</f>
-        <v>0.12105697977168035</v>
-      </c>
-      <c r="Q33" s="121"/>
-      <c r="R33" s="147">
-        <f>(t_data!$P$6)</f>
-        <v>131</v>
-      </c>
-      <c r="S33" s="148"/>
-      <c r="T33" s="117">
-        <f>(t_data!$O$6)</f>
-        <v>9671</v>
-      </c>
-      <c r="U33" s="118"/>
-      <c r="V33" s="118"/>
-      <c r="W33" s="118"/>
-      <c r="X33" s="121">
+      <c r="S33" s="98"/>
+      <c r="T33" s="99">
+        <f>(t_data!$O$7)</f>
+        <v>9555</v>
+      </c>
+      <c r="U33" s="100"/>
+      <c r="V33" s="100"/>
+      <c r="W33" s="100"/>
+      <c r="X33" s="103">
         <f>(T33/T5)</f>
-        <v>0.12068384600985836</v>
-      </c>
-      <c r="Y33" s="121"/>
-      <c r="Z33" s="147">
-        <f>(t_data!$P$6)</f>
-        <v>131</v>
-      </c>
-      <c r="AA33" s="148"/>
-      <c r="AB33" s="117">
-        <f>(t_data!$O$6)</f>
-        <v>9671</v>
-      </c>
-      <c r="AC33" s="118"/>
-      <c r="AD33" s="118"/>
-      <c r="AE33" s="118"/>
-      <c r="AF33" s="121">
+        <v>0.11923628876271292</v>
+      </c>
+      <c r="Y33" s="103"/>
+      <c r="Z33" s="97">
+        <f>(t_data!$P$7)</f>
+        <v>-116</v>
+      </c>
+      <c r="AA33" s="98"/>
+      <c r="AB33" s="99">
+        <f>(t_data!$O$8)</f>
+        <v>9657</v>
+      </c>
+      <c r="AC33" s="100"/>
+      <c r="AD33" s="100"/>
+      <c r="AE33" s="100"/>
+      <c r="AF33" s="103">
         <f>(AB33/AB5)</f>
-        <v>0.1184039765910037</v>
-      </c>
-      <c r="AG33" s="121"/>
-      <c r="AH33" s="147">
-        <f>(t_data!$P$6)</f>
-        <v>131</v>
-      </c>
-      <c r="AI33" s="148"/>
-      <c r="AJ33" s="117">
-        <f>(t_data!$O$6)</f>
-        <v>9671</v>
-      </c>
-      <c r="AK33" s="118"/>
-      <c r="AL33" s="118"/>
-      <c r="AM33" s="118"/>
-      <c r="AN33" s="121">
+        <v>0.11823257180636157</v>
+      </c>
+      <c r="AG33" s="103"/>
+      <c r="AH33" s="97">
+        <f>(t_data!$P$8)</f>
+        <v>102</v>
+      </c>
+      <c r="AI33" s="98"/>
+      <c r="AJ33" s="99">
+        <f>(t_data!$O$9)</f>
+        <v>9596</v>
+      </c>
+      <c r="AK33" s="100"/>
+      <c r="AL33" s="100"/>
+      <c r="AM33" s="100"/>
+      <c r="AN33" s="103">
         <f>(AJ33/AJ5)</f>
-        <v>0.11615840109540339</v>
-      </c>
-      <c r="AO33" s="121"/>
-      <c r="AP33" s="147">
-        <f>(t_data!$P$6)</f>
-        <v>131</v>
-      </c>
-      <c r="AQ33" s="148"/>
-      <c r="AR33" s="117">
-        <f>(t_data!$O$6)</f>
-        <v>9671</v>
-      </c>
-      <c r="AS33" s="118"/>
-      <c r="AT33" s="118"/>
-      <c r="AU33" s="118"/>
-      <c r="AV33" s="121">
+        <v>0.11525757593956064</v>
+      </c>
+      <c r="AO33" s="103"/>
+      <c r="AP33" s="97">
+        <f>(t_data!$P$9)</f>
+        <v>-61</v>
+      </c>
+      <c r="AQ33" s="98"/>
+      <c r="AR33" s="99">
+        <f>(t_data!$O$10)</f>
+        <v>9432</v>
+      </c>
+      <c r="AS33" s="100"/>
+      <c r="AT33" s="100"/>
+      <c r="AU33" s="100"/>
+      <c r="AV33" s="103">
         <f>(AR33/AR5)</f>
-        <v>0.11550220948286158</v>
-      </c>
-      <c r="AW33" s="121"/>
-      <c r="AX33" s="147">
-        <f>(t_data!$P$6)</f>
-        <v>131</v>
-      </c>
-      <c r="AY33" s="147"/>
-      <c r="AZ33" s="88">
+        <v>0.11264779648871372</v>
+      </c>
+      <c r="AW33" s="103"/>
+      <c r="AX33" s="97">
+        <f>(t_data!$P$10)</f>
+        <v>-164</v>
+      </c>
+      <c r="AY33" s="97"/>
+      <c r="AZ33" s="176">
         <f>(t_data!P11)</f>
         <v>-108</v>
       </c>
-      <c r="BA33" s="89"/>
-      <c r="BB33" s="89"/>
-      <c r="BC33" s="89"/>
-      <c r="BD33" s="89"/>
-      <c r="BE33" s="89"/>
-      <c r="BF33" s="90"/>
+      <c r="BA33" s="177"/>
+      <c r="BB33" s="177"/>
+      <c r="BC33" s="177"/>
+      <c r="BD33" s="177"/>
+      <c r="BE33" s="177"/>
+      <c r="BF33" s="178"/>
     </row>
     <row r="34" spans="1:58">
-      <c r="A34" s="123"/>
-      <c r="B34" s="123"/>
-      <c r="C34" s="123"/>
-      <c r="D34" s="119"/>
-      <c r="E34" s="120"/>
-      <c r="F34" s="120"/>
-      <c r="G34" s="120"/>
-      <c r="H34" s="122"/>
-      <c r="I34" s="122"/>
-      <c r="J34" s="149">
+      <c r="A34" s="105"/>
+      <c r="B34" s="105"/>
+      <c r="C34" s="105"/>
+      <c r="D34" s="101"/>
+      <c r="E34" s="102"/>
+      <c r="F34" s="102"/>
+      <c r="G34" s="102"/>
+      <c r="H34" s="104"/>
+      <c r="I34" s="104"/>
+      <c r="J34" s="64">
+        <f>(t_data!$Q$5)</f>
+        <v>4.2964906526730129E-2</v>
+      </c>
+      <c r="K34" s="65"/>
+      <c r="L34" s="101"/>
+      <c r="M34" s="102"/>
+      <c r="N34" s="102"/>
+      <c r="O34" s="102"/>
+      <c r="P34" s="104"/>
+      <c r="Q34" s="104"/>
+      <c r="R34" s="64">
         <f>(t_data!$Q$6)</f>
         <v>1.3731656184486463E-2</v>
       </c>
-      <c r="K34" s="150"/>
-      <c r="L34" s="119"/>
-      <c r="M34" s="120"/>
-      <c r="N34" s="120"/>
-      <c r="O34" s="120"/>
-      <c r="P34" s="122"/>
-      <c r="Q34" s="122"/>
-      <c r="R34" s="149">
-        <f>(t_data!$Q$6)</f>
-        <v>1.3731656184486463E-2</v>
-      </c>
-      <c r="S34" s="150"/>
-      <c r="T34" s="119"/>
-      <c r="U34" s="120"/>
-      <c r="V34" s="120"/>
-      <c r="W34" s="120"/>
-      <c r="X34" s="122"/>
-      <c r="Y34" s="122"/>
-      <c r="Z34" s="149">
-        <f>(t_data!$Q$6)</f>
-        <v>1.3731656184486463E-2</v>
-      </c>
-      <c r="AA34" s="150"/>
-      <c r="AB34" s="119"/>
-      <c r="AC34" s="120"/>
-      <c r="AD34" s="120"/>
-      <c r="AE34" s="120"/>
-      <c r="AF34" s="122"/>
-      <c r="AG34" s="122"/>
-      <c r="AH34" s="149">
-        <f>(t_data!$Q$6)</f>
-        <v>1.3731656184486463E-2</v>
-      </c>
-      <c r="AI34" s="150"/>
-      <c r="AJ34" s="119"/>
-      <c r="AK34" s="120"/>
-      <c r="AL34" s="120"/>
-      <c r="AM34" s="120"/>
-      <c r="AN34" s="122"/>
-      <c r="AO34" s="122"/>
-      <c r="AP34" s="149">
-        <f>(t_data!$Q$6)</f>
-        <v>1.3731656184486463E-2</v>
-      </c>
-      <c r="AQ34" s="150"/>
-      <c r="AR34" s="119"/>
-      <c r="AS34" s="120"/>
-      <c r="AT34" s="120"/>
-      <c r="AU34" s="120"/>
-      <c r="AV34" s="122"/>
-      <c r="AW34" s="122"/>
-      <c r="AX34" s="149">
-        <f>(t_data!$Q$6)</f>
-        <v>1.3731656184486463E-2</v>
-      </c>
-      <c r="AY34" s="149"/>
-      <c r="AZ34" s="91">
+      <c r="S34" s="65"/>
+      <c r="T34" s="101"/>
+      <c r="U34" s="102"/>
+      <c r="V34" s="102"/>
+      <c r="W34" s="102"/>
+      <c r="X34" s="104"/>
+      <c r="Y34" s="104"/>
+      <c r="Z34" s="64">
+        <f>(t_data!$Q$7)</f>
+        <v>-1.1994623099989665E-2</v>
+      </c>
+      <c r="AA34" s="65"/>
+      <c r="AB34" s="101"/>
+      <c r="AC34" s="102"/>
+      <c r="AD34" s="102"/>
+      <c r="AE34" s="102"/>
+      <c r="AF34" s="104"/>
+      <c r="AG34" s="104"/>
+      <c r="AH34" s="64">
+        <f>(t_data!$Q$8)</f>
+        <v>1.0675039246467843E-2</v>
+      </c>
+      <c r="AI34" s="65"/>
+      <c r="AJ34" s="101"/>
+      <c r="AK34" s="102"/>
+      <c r="AL34" s="102"/>
+      <c r="AM34" s="102"/>
+      <c r="AN34" s="104"/>
+      <c r="AO34" s="104"/>
+      <c r="AP34" s="64">
+        <f>(t_data!$Q$9)</f>
+        <v>-6.3166614890752815E-3</v>
+      </c>
+      <c r="AQ34" s="65"/>
+      <c r="AR34" s="101"/>
+      <c r="AS34" s="102"/>
+      <c r="AT34" s="102"/>
+      <c r="AU34" s="102"/>
+      <c r="AV34" s="104"/>
+      <c r="AW34" s="104"/>
+      <c r="AX34" s="64">
+        <f>(t_data!$Q$10)</f>
+        <v>-1.7090454355981666E-2</v>
+      </c>
+      <c r="AY34" s="64"/>
+      <c r="AZ34" s="179">
         <f>(t_data!Q11)</f>
         <v>-1.132075471698113E-2</v>
       </c>
-      <c r="BA34" s="92"/>
-      <c r="BB34" s="92"/>
-      <c r="BC34" s="92"/>
-      <c r="BD34" s="92"/>
-      <c r="BE34" s="92"/>
-      <c r="BF34" s="93"/>
+      <c r="BA34" s="180"/>
+      <c r="BB34" s="180"/>
+      <c r="BC34" s="180"/>
+      <c r="BD34" s="180"/>
+      <c r="BE34" s="180"/>
+      <c r="BF34" s="181"/>
     </row>
     <row r="35" spans="1:58">
       <c r="A35" s="32"/>
@@ -20082,59 +20081,59 @@
       <c r="BF35" s="27"/>
     </row>
     <row r="36" spans="1:58">
-      <c r="A36" s="136" t="s">
+      <c r="A36" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="136"/>
-      <c r="C36" s="136"/>
-      <c r="D36" s="136"/>
-      <c r="E36" s="136"/>
-      <c r="F36" s="136"/>
-      <c r="G36" s="136"/>
-      <c r="H36" s="136"/>
-      <c r="I36" s="136"/>
-      <c r="J36" s="136"/>
-      <c r="K36" s="136"/>
-      <c r="L36" s="136"/>
-      <c r="M36" s="136"/>
-      <c r="N36" s="136"/>
-      <c r="O36" s="136"/>
-      <c r="P36" s="136"/>
-      <c r="Q36" s="136"/>
-      <c r="R36" s="136"/>
-      <c r="S36" s="136"/>
-      <c r="T36" s="136"/>
-      <c r="U36" s="136"/>
-      <c r="V36" s="136"/>
-      <c r="W36" s="136"/>
-      <c r="X36" s="136"/>
-      <c r="Y36" s="136"/>
-      <c r="Z36" s="136"/>
-      <c r="AA36" s="136"/>
-      <c r="AB36" s="136"/>
-      <c r="AC36" s="136"/>
-      <c r="AD36" s="136"/>
-      <c r="AE36" s="136"/>
-      <c r="AF36" s="136"/>
-      <c r="AG36" s="136"/>
-      <c r="AH36" s="136"/>
-      <c r="AI36" s="136"/>
-      <c r="AJ36" s="136"/>
-      <c r="AK36" s="136"/>
-      <c r="AL36" s="136"/>
-      <c r="AM36" s="136"/>
-      <c r="AN36" s="136"/>
-      <c r="AO36" s="136"/>
-      <c r="AP36" s="136"/>
-      <c r="AQ36" s="136"/>
-      <c r="AR36" s="136"/>
-      <c r="AS36" s="136"/>
-      <c r="AT36" s="136"/>
-      <c r="AU36" s="136"/>
-      <c r="AV36" s="136"/>
-      <c r="AW36" s="136"/>
-      <c r="AX36" s="136"/>
-      <c r="AY36" s="136"/>
+      <c r="B36" s="96"/>
+      <c r="C36" s="96"/>
+      <c r="D36" s="96"/>
+      <c r="E36" s="96"/>
+      <c r="F36" s="96"/>
+      <c r="G36" s="96"/>
+      <c r="H36" s="96"/>
+      <c r="I36" s="96"/>
+      <c r="J36" s="96"/>
+      <c r="K36" s="96"/>
+      <c r="L36" s="96"/>
+      <c r="M36" s="96"/>
+      <c r="N36" s="96"/>
+      <c r="O36" s="96"/>
+      <c r="P36" s="96"/>
+      <c r="Q36" s="96"/>
+      <c r="R36" s="96"/>
+      <c r="S36" s="96"/>
+      <c r="T36" s="96"/>
+      <c r="U36" s="96"/>
+      <c r="V36" s="96"/>
+      <c r="W36" s="96"/>
+      <c r="X36" s="96"/>
+      <c r="Y36" s="96"/>
+      <c r="Z36" s="96"/>
+      <c r="AA36" s="96"/>
+      <c r="AB36" s="96"/>
+      <c r="AC36" s="96"/>
+      <c r="AD36" s="96"/>
+      <c r="AE36" s="96"/>
+      <c r="AF36" s="96"/>
+      <c r="AG36" s="96"/>
+      <c r="AH36" s="96"/>
+      <c r="AI36" s="96"/>
+      <c r="AJ36" s="96"/>
+      <c r="AK36" s="96"/>
+      <c r="AL36" s="96"/>
+      <c r="AM36" s="96"/>
+      <c r="AN36" s="96"/>
+      <c r="AO36" s="96"/>
+      <c r="AP36" s="96"/>
+      <c r="AQ36" s="96"/>
+      <c r="AR36" s="96"/>
+      <c r="AS36" s="96"/>
+      <c r="AT36" s="96"/>
+      <c r="AU36" s="96"/>
+      <c r="AV36" s="96"/>
+      <c r="AW36" s="96"/>
+      <c r="AX36" s="96"/>
+      <c r="AY36" s="96"/>
       <c r="AZ36" s="27"/>
       <c r="BA36" s="27"/>
       <c r="BB36" s="27"/>
@@ -20144,453 +20143,453 @@
       <c r="BF36" s="27"/>
     </row>
     <row r="37" spans="1:58">
-      <c r="A37" s="126"/>
-      <c r="B37" s="145"/>
-      <c r="C37" s="146"/>
-      <c r="D37" s="124" t="str">
+      <c r="A37" s="50"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="48" t="str">
         <f>(t_data!$B$5)</f>
         <v>2020-08-01</v>
       </c>
-      <c r="E37" s="125"/>
-      <c r="F37" s="125"/>
-      <c r="G37" s="125"/>
-      <c r="H37" s="125"/>
-      <c r="I37" s="125"/>
-      <c r="J37" s="125"/>
-      <c r="K37" s="125"/>
-      <c r="L37" s="124" t="str">
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="49"/>
+      <c r="K37" s="49"/>
+      <c r="L37" s="48" t="str">
         <f>(t_data!$B$6)</f>
         <v>2021-08-01</v>
       </c>
-      <c r="M37" s="125"/>
-      <c r="N37" s="125"/>
-      <c r="O37" s="125"/>
-      <c r="P37" s="125"/>
-      <c r="Q37" s="125"/>
-      <c r="R37" s="125"/>
-      <c r="S37" s="125"/>
-      <c r="T37" s="124" t="str">
+      <c r="M37" s="49"/>
+      <c r="N37" s="49"/>
+      <c r="O37" s="49"/>
+      <c r="P37" s="49"/>
+      <c r="Q37" s="49"/>
+      <c r="R37" s="49"/>
+      <c r="S37" s="49"/>
+      <c r="T37" s="48" t="str">
         <f>(t_data!$B$7)</f>
         <v>2022-08-01</v>
       </c>
-      <c r="U37" s="125"/>
-      <c r="V37" s="125"/>
-      <c r="W37" s="125"/>
-      <c r="X37" s="125"/>
-      <c r="Y37" s="125"/>
-      <c r="Z37" s="125"/>
-      <c r="AA37" s="125"/>
-      <c r="AB37" s="124" t="str">
+      <c r="U37" s="49"/>
+      <c r="V37" s="49"/>
+      <c r="W37" s="49"/>
+      <c r="X37" s="49"/>
+      <c r="Y37" s="49"/>
+      <c r="Z37" s="49"/>
+      <c r="AA37" s="49"/>
+      <c r="AB37" s="48" t="str">
         <f>(t_data!$B$8)</f>
         <v>2023-08-01</v>
       </c>
-      <c r="AC37" s="125"/>
-      <c r="AD37" s="125"/>
-      <c r="AE37" s="125"/>
-      <c r="AF37" s="125"/>
-      <c r="AG37" s="125"/>
-      <c r="AH37" s="125"/>
-      <c r="AI37" s="125"/>
-      <c r="AJ37" s="124" t="str">
+      <c r="AC37" s="49"/>
+      <c r="AD37" s="49"/>
+      <c r="AE37" s="49"/>
+      <c r="AF37" s="49"/>
+      <c r="AG37" s="49"/>
+      <c r="AH37" s="49"/>
+      <c r="AI37" s="49"/>
+      <c r="AJ37" s="48" t="str">
         <f>(t_data!$B$9)</f>
         <v>2024-08-01</v>
       </c>
-      <c r="AK37" s="125"/>
-      <c r="AL37" s="125"/>
-      <c r="AM37" s="125"/>
-      <c r="AN37" s="125"/>
-      <c r="AO37" s="125"/>
-      <c r="AP37" s="125"/>
-      <c r="AQ37" s="125"/>
-      <c r="AR37" s="124" t="str">
+      <c r="AK37" s="49"/>
+      <c r="AL37" s="49"/>
+      <c r="AM37" s="49"/>
+      <c r="AN37" s="49"/>
+      <c r="AO37" s="49"/>
+      <c r="AP37" s="49"/>
+      <c r="AQ37" s="49"/>
+      <c r="AR37" s="48" t="str">
         <f>(t_data!$B$10)</f>
         <v>2025-08-01</v>
       </c>
-      <c r="AS37" s="125"/>
-      <c r="AT37" s="125"/>
-      <c r="AU37" s="125"/>
-      <c r="AV37" s="125"/>
-      <c r="AW37" s="125"/>
-      <c r="AX37" s="125"/>
-      <c r="AY37" s="126"/>
-      <c r="AZ37" s="97" t="s">
-        <v>228</v>
-      </c>
-      <c r="BA37" s="145"/>
-      <c r="BB37" s="145"/>
-      <c r="BC37" s="145"/>
-      <c r="BD37" s="145"/>
-      <c r="BE37" s="145"/>
-      <c r="BF37" s="146"/>
+      <c r="AS37" s="49"/>
+      <c r="AT37" s="49"/>
+      <c r="AU37" s="49"/>
+      <c r="AV37" s="49"/>
+      <c r="AW37" s="49"/>
+      <c r="AX37" s="49"/>
+      <c r="AY37" s="50"/>
+      <c r="AZ37" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="BA37" s="75"/>
+      <c r="BB37" s="75"/>
+      <c r="BC37" s="75"/>
+      <c r="BD37" s="75"/>
+      <c r="BE37" s="75"/>
+      <c r="BF37" s="76"/>
     </row>
     <row r="38" spans="1:58">
-      <c r="A38" s="161" t="s">
+      <c r="A38" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="B38" s="162"/>
-      <c r="C38" s="163"/>
-      <c r="D38" s="167">
+      <c r="B38" s="91"/>
+      <c r="C38" s="92"/>
+      <c r="D38" s="51">
         <f>(I38+I39)</f>
         <v>277</v>
       </c>
-      <c r="E38" s="159"/>
-      <c r="F38" s="159"/>
-      <c r="G38" s="159"/>
+      <c r="E38" s="52"/>
+      <c r="F38" s="52"/>
+      <c r="G38" s="52"/>
       <c r="H38" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="I38" s="159">
+      <c r="I38" s="52">
         <f>(g_data!$E$26)</f>
         <v>844</v>
       </c>
-      <c r="J38" s="159"/>
-      <c r="K38" s="160"/>
-      <c r="L38" s="167">
+      <c r="J38" s="52"/>
+      <c r="K38" s="56"/>
+      <c r="L38" s="51">
         <f>(Q38+Q39)</f>
         <v>169</v>
       </c>
-      <c r="M38" s="159"/>
-      <c r="N38" s="159"/>
-      <c r="O38" s="159"/>
+      <c r="M38" s="52"/>
+      <c r="N38" s="52"/>
+      <c r="O38" s="52"/>
       <c r="P38" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="Q38" s="159">
+      <c r="Q38" s="52">
         <f>(g_data!$E$27)</f>
         <v>731</v>
       </c>
-      <c r="R38" s="159"/>
-      <c r="S38" s="160"/>
-      <c r="T38" s="167">
+      <c r="R38" s="52"/>
+      <c r="S38" s="56"/>
+      <c r="T38" s="51">
         <f>(Y38+Y39)</f>
         <v>74</v>
       </c>
-      <c r="U38" s="159"/>
-      <c r="V38" s="159"/>
-      <c r="W38" s="159"/>
+      <c r="U38" s="52"/>
+      <c r="V38" s="52"/>
+      <c r="W38" s="52"/>
       <c r="X38" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="Y38" s="159">
+      <c r="Y38" s="52">
         <f>(g_data!$E$28)</f>
         <v>744</v>
       </c>
-      <c r="Z38" s="159"/>
-      <c r="AA38" s="160"/>
-      <c r="AB38" s="167">
+      <c r="Z38" s="52"/>
+      <c r="AA38" s="56"/>
+      <c r="AB38" s="51">
         <f>(AG38+AG39)</f>
         <v>-11</v>
       </c>
-      <c r="AC38" s="159"/>
-      <c r="AD38" s="159"/>
-      <c r="AE38" s="159"/>
+      <c r="AC38" s="52"/>
+      <c r="AD38" s="52"/>
+      <c r="AE38" s="52"/>
       <c r="AF38" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="AG38" s="159">
+      <c r="AG38" s="52">
         <f>(g_data!$E$29)</f>
         <v>741</v>
       </c>
-      <c r="AH38" s="159"/>
-      <c r="AI38" s="160"/>
-      <c r="AJ38" s="167">
+      <c r="AH38" s="52"/>
+      <c r="AI38" s="56"/>
+      <c r="AJ38" s="51">
         <f>(AO38+AO39)</f>
         <v>20</v>
       </c>
-      <c r="AK38" s="159"/>
-      <c r="AL38" s="159"/>
-      <c r="AM38" s="159"/>
+      <c r="AK38" s="52"/>
+      <c r="AL38" s="52"/>
+      <c r="AM38" s="52"/>
       <c r="AN38" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="AO38" s="159">
+      <c r="AO38" s="52">
         <f>(g_data!$E$30)</f>
         <v>692</v>
       </c>
-      <c r="AP38" s="159"/>
-      <c r="AQ38" s="160"/>
-      <c r="AR38" s="167">
+      <c r="AP38" s="52"/>
+      <c r="AQ38" s="56"/>
+      <c r="AR38" s="51">
         <f>(AW38+AW39)</f>
         <v>53</v>
       </c>
-      <c r="AS38" s="159"/>
-      <c r="AT38" s="159"/>
-      <c r="AU38" s="159"/>
+      <c r="AS38" s="52"/>
+      <c r="AT38" s="52"/>
+      <c r="AU38" s="52"/>
       <c r="AV38" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="AW38" s="159">
+      <c r="AW38" s="52">
         <f>(g_data!$E$31)</f>
         <v>694</v>
       </c>
-      <c r="AX38" s="159"/>
-      <c r="AY38" s="159"/>
-      <c r="AZ38" s="68">
+      <c r="AX38" s="52"/>
+      <c r="AY38" s="52"/>
+      <c r="AZ38" s="77">
         <f>(t_data!Z11)</f>
         <v>305</v>
       </c>
-      <c r="BA38" s="69"/>
-      <c r="BB38" s="69"/>
-      <c r="BC38" s="69"/>
-      <c r="BD38" s="69"/>
-      <c r="BE38" s="69"/>
-      <c r="BF38" s="70"/>
+      <c r="BA38" s="78"/>
+      <c r="BB38" s="78"/>
+      <c r="BC38" s="78"/>
+      <c r="BD38" s="78"/>
+      <c r="BE38" s="78"/>
+      <c r="BF38" s="79"/>
     </row>
     <row r="39" spans="1:58">
-      <c r="A39" s="164"/>
-      <c r="B39" s="165"/>
-      <c r="C39" s="166"/>
-      <c r="D39" s="168"/>
-      <c r="E39" s="157"/>
-      <c r="F39" s="157"/>
-      <c r="G39" s="157"/>
+      <c r="A39" s="93"/>
+      <c r="B39" s="94"/>
+      <c r="C39" s="95"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="54"/>
       <c r="H39" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="I39" s="157">
+      <c r="I39" s="54">
         <f>(g_data!$F$26)</f>
         <v>-567</v>
       </c>
-      <c r="J39" s="157"/>
-      <c r="K39" s="158"/>
-      <c r="L39" s="168"/>
-      <c r="M39" s="157"/>
-      <c r="N39" s="157"/>
-      <c r="O39" s="157"/>
+      <c r="J39" s="54"/>
+      <c r="K39" s="55"/>
+      <c r="L39" s="53"/>
+      <c r="M39" s="54"/>
+      <c r="N39" s="54"/>
+      <c r="O39" s="54"/>
       <c r="P39" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="Q39" s="157">
+      <c r="Q39" s="54">
         <f>(g_data!$F$27)</f>
         <v>-562</v>
       </c>
-      <c r="R39" s="157"/>
-      <c r="S39" s="158"/>
-      <c r="T39" s="168"/>
-      <c r="U39" s="157"/>
-      <c r="V39" s="157"/>
-      <c r="W39" s="157"/>
+      <c r="R39" s="54"/>
+      <c r="S39" s="55"/>
+      <c r="T39" s="53"/>
+      <c r="U39" s="54"/>
+      <c r="V39" s="54"/>
+      <c r="W39" s="54"/>
       <c r="X39" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="Y39" s="157">
+      <c r="Y39" s="54">
         <f>(g_data!$F$28)</f>
         <v>-670</v>
       </c>
-      <c r="Z39" s="157"/>
-      <c r="AA39" s="158"/>
-      <c r="AB39" s="168"/>
-      <c r="AC39" s="157"/>
-      <c r="AD39" s="157"/>
-      <c r="AE39" s="157"/>
+      <c r="Z39" s="54"/>
+      <c r="AA39" s="55"/>
+      <c r="AB39" s="53"/>
+      <c r="AC39" s="54"/>
+      <c r="AD39" s="54"/>
+      <c r="AE39" s="54"/>
       <c r="AF39" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="AG39" s="157">
+      <c r="AG39" s="54">
         <f>(g_data!$F$29)</f>
         <v>-752</v>
       </c>
-      <c r="AH39" s="157"/>
-      <c r="AI39" s="158"/>
-      <c r="AJ39" s="168"/>
-      <c r="AK39" s="157"/>
-      <c r="AL39" s="157"/>
-      <c r="AM39" s="157"/>
+      <c r="AH39" s="54"/>
+      <c r="AI39" s="55"/>
+      <c r="AJ39" s="53"/>
+      <c r="AK39" s="54"/>
+      <c r="AL39" s="54"/>
+      <c r="AM39" s="54"/>
       <c r="AN39" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="AO39" s="157">
+      <c r="AO39" s="54">
         <f>(g_data!$F$30)</f>
         <v>-672</v>
       </c>
-      <c r="AP39" s="157"/>
-      <c r="AQ39" s="158"/>
-      <c r="AR39" s="168"/>
-      <c r="AS39" s="157"/>
-      <c r="AT39" s="157"/>
-      <c r="AU39" s="157"/>
+      <c r="AP39" s="54"/>
+      <c r="AQ39" s="55"/>
+      <c r="AR39" s="53"/>
+      <c r="AS39" s="54"/>
+      <c r="AT39" s="54"/>
+      <c r="AU39" s="54"/>
       <c r="AV39" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="AW39" s="157">
+      <c r="AW39" s="54">
         <f>(g_data!$F$31)</f>
         <v>-641</v>
       </c>
-      <c r="AX39" s="157"/>
-      <c r="AY39" s="157"/>
-      <c r="AZ39" s="71"/>
-      <c r="BA39" s="72"/>
-      <c r="BB39" s="72"/>
-      <c r="BC39" s="72"/>
-      <c r="BD39" s="72"/>
-      <c r="BE39" s="72"/>
-      <c r="BF39" s="73"/>
+      <c r="AX39" s="54"/>
+      <c r="AY39" s="54"/>
+      <c r="AZ39" s="159"/>
+      <c r="BA39" s="160"/>
+      <c r="BB39" s="160"/>
+      <c r="BC39" s="160"/>
+      <c r="BD39" s="160"/>
+      <c r="BE39" s="160"/>
+      <c r="BF39" s="161"/>
     </row>
     <row r="40" spans="1:58" ht="19.5" thickBot="1">
-      <c r="A40" s="151" t="s">
+      <c r="A40" s="87" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="152"/>
-      <c r="C40" s="153"/>
-      <c r="D40" s="154">
+      <c r="B40" s="88"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="45">
         <f>(g_data!$G$26)</f>
         <v>1882</v>
       </c>
-      <c r="E40" s="155"/>
-      <c r="F40" s="155"/>
-      <c r="G40" s="155"/>
-      <c r="H40" s="155"/>
-      <c r="I40" s="155"/>
-      <c r="J40" s="155"/>
-      <c r="K40" s="156"/>
-      <c r="L40" s="154">
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="47"/>
+      <c r="L40" s="45">
         <f>(g_data!$G$27)</f>
         <v>442</v>
       </c>
-      <c r="M40" s="155"/>
-      <c r="N40" s="155"/>
-      <c r="O40" s="155"/>
-      <c r="P40" s="155"/>
-      <c r="Q40" s="155"/>
-      <c r="R40" s="155"/>
-      <c r="S40" s="156"/>
-      <c r="T40" s="154">
+      <c r="M40" s="46"/>
+      <c r="N40" s="46"/>
+      <c r="O40" s="46"/>
+      <c r="P40" s="46"/>
+      <c r="Q40" s="46"/>
+      <c r="R40" s="46"/>
+      <c r="S40" s="47"/>
+      <c r="T40" s="45">
         <f>(g_data!$G$28)</f>
         <v>173</v>
       </c>
-      <c r="U40" s="155"/>
-      <c r="V40" s="155"/>
-      <c r="W40" s="155"/>
-      <c r="X40" s="155"/>
-      <c r="Y40" s="155"/>
-      <c r="Z40" s="155"/>
-      <c r="AA40" s="156"/>
-      <c r="AB40" s="154">
+      <c r="U40" s="46"/>
+      <c r="V40" s="46"/>
+      <c r="W40" s="46"/>
+      <c r="X40" s="46"/>
+      <c r="Y40" s="46"/>
+      <c r="Z40" s="46"/>
+      <c r="AA40" s="47"/>
+      <c r="AB40" s="45">
         <f>(g_data!$G$29)</f>
         <v>1554</v>
       </c>
-      <c r="AC40" s="155"/>
-      <c r="AD40" s="155"/>
-      <c r="AE40" s="155"/>
-      <c r="AF40" s="155"/>
-      <c r="AG40" s="155"/>
-      <c r="AH40" s="155"/>
-      <c r="AI40" s="156"/>
-      <c r="AJ40" s="154">
+      <c r="AC40" s="46"/>
+      <c r="AD40" s="46"/>
+      <c r="AE40" s="46"/>
+      <c r="AF40" s="46"/>
+      <c r="AG40" s="46"/>
+      <c r="AH40" s="46"/>
+      <c r="AI40" s="47"/>
+      <c r="AJ40" s="45">
         <f>(g_data!$G$30)</f>
         <v>1559</v>
       </c>
-      <c r="AK40" s="155"/>
-      <c r="AL40" s="155"/>
-      <c r="AM40" s="155"/>
-      <c r="AN40" s="155"/>
-      <c r="AO40" s="155"/>
-      <c r="AP40" s="155"/>
-      <c r="AQ40" s="156"/>
-      <c r="AR40" s="154">
+      <c r="AK40" s="46"/>
+      <c r="AL40" s="46"/>
+      <c r="AM40" s="46"/>
+      <c r="AN40" s="46"/>
+      <c r="AO40" s="46"/>
+      <c r="AP40" s="46"/>
+      <c r="AQ40" s="47"/>
+      <c r="AR40" s="45">
         <f>(g_data!$G$31)</f>
         <v>420</v>
       </c>
-      <c r="AS40" s="155"/>
-      <c r="AT40" s="155"/>
-      <c r="AU40" s="155"/>
-      <c r="AV40" s="155"/>
-      <c r="AW40" s="155"/>
-      <c r="AX40" s="155"/>
-      <c r="AY40" s="155"/>
-      <c r="AZ40" s="68">
+      <c r="AS40" s="46"/>
+      <c r="AT40" s="46"/>
+      <c r="AU40" s="46"/>
+      <c r="AV40" s="46"/>
+      <c r="AW40" s="46"/>
+      <c r="AX40" s="46"/>
+      <c r="AY40" s="46"/>
+      <c r="AZ40" s="77">
         <f>(t_data!AB11)</f>
         <v>4148</v>
       </c>
-      <c r="BA40" s="69"/>
-      <c r="BB40" s="69"/>
-      <c r="BC40" s="69"/>
-      <c r="BD40" s="69"/>
-      <c r="BE40" s="69"/>
-      <c r="BF40" s="70"/>
+      <c r="BA40" s="78"/>
+      <c r="BB40" s="78"/>
+      <c r="BC40" s="78"/>
+      <c r="BD40" s="78"/>
+      <c r="BE40" s="78"/>
+      <c r="BF40" s="79"/>
     </row>
     <row r="41" spans="1:58" ht="19.5" thickTop="1">
-      <c r="A41" s="177" t="s">
+      <c r="A41" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="178"/>
-      <c r="C41" s="179"/>
-      <c r="D41" s="180">
+      <c r="B41" s="40"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="42">
         <f>(D38+D40)</f>
         <v>2159</v>
       </c>
-      <c r="E41" s="181"/>
-      <c r="F41" s="181"/>
-      <c r="G41" s="181"/>
-      <c r="H41" s="181"/>
-      <c r="I41" s="181"/>
-      <c r="J41" s="181"/>
-      <c r="K41" s="182"/>
-      <c r="L41" s="180">
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="44"/>
+      <c r="L41" s="42">
         <f>(L38+L40)</f>
         <v>611</v>
       </c>
-      <c r="M41" s="181"/>
-      <c r="N41" s="181"/>
-      <c r="O41" s="181"/>
-      <c r="P41" s="181"/>
-      <c r="Q41" s="181"/>
-      <c r="R41" s="181"/>
-      <c r="S41" s="182"/>
-      <c r="T41" s="180">
+      <c r="M41" s="43"/>
+      <c r="N41" s="43"/>
+      <c r="O41" s="43"/>
+      <c r="P41" s="43"/>
+      <c r="Q41" s="43"/>
+      <c r="R41" s="43"/>
+      <c r="S41" s="44"/>
+      <c r="T41" s="42">
         <f>(T38+T40)</f>
         <v>247</v>
       </c>
-      <c r="U41" s="181"/>
-      <c r="V41" s="181"/>
-      <c r="W41" s="181"/>
-      <c r="X41" s="181"/>
-      <c r="Y41" s="181"/>
-      <c r="Z41" s="181"/>
-      <c r="AA41" s="182"/>
-      <c r="AB41" s="180">
+      <c r="U41" s="43"/>
+      <c r="V41" s="43"/>
+      <c r="W41" s="43"/>
+      <c r="X41" s="43"/>
+      <c r="Y41" s="43"/>
+      <c r="Z41" s="43"/>
+      <c r="AA41" s="44"/>
+      <c r="AB41" s="42">
         <f>(AB38+AB40)</f>
         <v>1543</v>
       </c>
-      <c r="AC41" s="181"/>
-      <c r="AD41" s="181"/>
-      <c r="AE41" s="181"/>
-      <c r="AF41" s="181"/>
-      <c r="AG41" s="181"/>
-      <c r="AH41" s="181"/>
-      <c r="AI41" s="182"/>
-      <c r="AJ41" s="180">
+      <c r="AC41" s="43"/>
+      <c r="AD41" s="43"/>
+      <c r="AE41" s="43"/>
+      <c r="AF41" s="43"/>
+      <c r="AG41" s="43"/>
+      <c r="AH41" s="43"/>
+      <c r="AI41" s="44"/>
+      <c r="AJ41" s="42">
         <f>(AJ38+AJ40)</f>
         <v>1579</v>
       </c>
-      <c r="AK41" s="181"/>
-      <c r="AL41" s="181"/>
-      <c r="AM41" s="181"/>
-      <c r="AN41" s="181"/>
-      <c r="AO41" s="181"/>
-      <c r="AP41" s="181"/>
-      <c r="AQ41" s="182"/>
-      <c r="AR41" s="180">
+      <c r="AK41" s="43"/>
+      <c r="AL41" s="43"/>
+      <c r="AM41" s="43"/>
+      <c r="AN41" s="43"/>
+      <c r="AO41" s="43"/>
+      <c r="AP41" s="43"/>
+      <c r="AQ41" s="44"/>
+      <c r="AR41" s="42">
         <f>(AR38+AR40)</f>
         <v>473</v>
       </c>
-      <c r="AS41" s="181"/>
-      <c r="AT41" s="181"/>
-      <c r="AU41" s="181"/>
-      <c r="AV41" s="181"/>
-      <c r="AW41" s="181"/>
-      <c r="AX41" s="181"/>
-      <c r="AY41" s="181"/>
-      <c r="AZ41" s="50">
+      <c r="AS41" s="43"/>
+      <c r="AT41" s="43"/>
+      <c r="AU41" s="43"/>
+      <c r="AV41" s="43"/>
+      <c r="AW41" s="43"/>
+      <c r="AX41" s="43"/>
+      <c r="AY41" s="43"/>
+      <c r="AZ41" s="141">
         <f>(AZ38+AZ40)</f>
         <v>4453</v>
       </c>
-      <c r="BA41" s="51"/>
-      <c r="BB41" s="51"/>
-      <c r="BC41" s="51"/>
-      <c r="BD41" s="51"/>
-      <c r="BE41" s="51"/>
-      <c r="BF41" s="52"/>
+      <c r="BA41" s="142"/>
+      <c r="BB41" s="142"/>
+      <c r="BC41" s="142"/>
+      <c r="BD41" s="142"/>
+      <c r="BE41" s="142"/>
+      <c r="BF41" s="143"/>
     </row>
     <row r="42" spans="1:58">
       <c r="A42" s="27"/>
@@ -20681,24 +20680,24 @@
       <c r="Z43" s="27"/>
       <c r="AA43" s="27"/>
       <c r="AB43" s="27"/>
-      <c r="AC43" s="173" t="s">
-        <v>232</v>
-      </c>
-      <c r="AD43" s="173"/>
-      <c r="AE43" s="173"/>
-      <c r="AF43" s="173"/>
-      <c r="AG43" s="173"/>
-      <c r="AH43" s="173"/>
-      <c r="AI43" s="173"/>
-      <c r="AJ43" s="173"/>
-      <c r="AK43" s="173"/>
-      <c r="AL43" s="173"/>
-      <c r="AM43" s="173"/>
-      <c r="AN43" s="173"/>
-      <c r="AO43" s="173"/>
-      <c r="AP43" s="173"/>
-      <c r="AQ43" s="173"/>
-      <c r="AR43" s="173"/>
+      <c r="AC43" s="59" t="s">
+        <v>231</v>
+      </c>
+      <c r="AD43" s="59"/>
+      <c r="AE43" s="59"/>
+      <c r="AF43" s="59"/>
+      <c r="AG43" s="59"/>
+      <c r="AH43" s="59"/>
+      <c r="AI43" s="59"/>
+      <c r="AJ43" s="59"/>
+      <c r="AK43" s="59"/>
+      <c r="AL43" s="59"/>
+      <c r="AM43" s="59"/>
+      <c r="AN43" s="59"/>
+      <c r="AO43" s="59"/>
+      <c r="AP43" s="59"/>
+      <c r="AQ43" s="59"/>
+      <c r="AR43" s="59"/>
       <c r="AS43" s="27"/>
       <c r="AT43" s="27"/>
       <c r="AU43" s="27"/>
@@ -21403,24 +21402,24 @@
       <c r="Z55" s="27"/>
       <c r="AA55" s="27"/>
       <c r="AB55" s="27"/>
-      <c r="AC55" s="173" t="s">
-        <v>233</v>
-      </c>
-      <c r="AD55" s="173"/>
-      <c r="AE55" s="173"/>
-      <c r="AF55" s="173"/>
-      <c r="AG55" s="173"/>
-      <c r="AH55" s="173"/>
-      <c r="AI55" s="173"/>
-      <c r="AJ55" s="173"/>
-      <c r="AK55" s="173"/>
-      <c r="AL55" s="173"/>
-      <c r="AM55" s="173"/>
-      <c r="AN55" s="173"/>
-      <c r="AO55" s="173"/>
-      <c r="AP55" s="173"/>
-      <c r="AQ55" s="173"/>
-      <c r="AR55" s="173"/>
+      <c r="AC55" s="59" t="s">
+        <v>232</v>
+      </c>
+      <c r="AD55" s="59"/>
+      <c r="AE55" s="59"/>
+      <c r="AF55" s="59"/>
+      <c r="AG55" s="59"/>
+      <c r="AH55" s="59"/>
+      <c r="AI55" s="59"/>
+      <c r="AJ55" s="59"/>
+      <c r="AK55" s="59"/>
+      <c r="AL55" s="59"/>
+      <c r="AM55" s="59"/>
+      <c r="AN55" s="59"/>
+      <c r="AO55" s="59"/>
+      <c r="AP55" s="59"/>
+      <c r="AQ55" s="59"/>
+      <c r="AR55" s="59"/>
       <c r="AS55" s="27"/>
       <c r="AT55" s="27"/>
       <c r="AU55" s="27"/>
@@ -22157,8 +22156,197 @@
       <c r="BF67" s="26"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" selectLockedCells="1"/>
+  <sheetProtection sheet="1" objects="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="213">
+    <mergeCell ref="BB1:BF1"/>
+    <mergeCell ref="AW1:BA1"/>
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="L8:P9"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="A1:P2"/>
+    <mergeCell ref="AZ41:BF41"/>
+    <mergeCell ref="AZ8:BF8"/>
+    <mergeCell ref="AZ9:BF9"/>
+    <mergeCell ref="BA10:BB10"/>
+    <mergeCell ref="BD5:BF5"/>
+    <mergeCell ref="BD6:BF6"/>
+    <mergeCell ref="BD7:BF7"/>
+    <mergeCell ref="BA7:BC7"/>
+    <mergeCell ref="BA6:BC6"/>
+    <mergeCell ref="AZ38:BF39"/>
+    <mergeCell ref="AZ5:BC5"/>
+    <mergeCell ref="AZ29:BF29"/>
+    <mergeCell ref="AZ30:BF30"/>
+    <mergeCell ref="AZ31:BF31"/>
+    <mergeCell ref="AZ32:BF32"/>
+    <mergeCell ref="AZ33:BF33"/>
+    <mergeCell ref="AZ34:BF34"/>
+    <mergeCell ref="AZ4:BF4"/>
+    <mergeCell ref="AZ28:BF28"/>
+    <mergeCell ref="AB7:AE7"/>
+    <mergeCell ref="AF7:AI7"/>
+    <mergeCell ref="AB8:AF9"/>
+    <mergeCell ref="AG8:AI8"/>
+    <mergeCell ref="AG9:AI9"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="D8:H9"/>
+    <mergeCell ref="T5:X6"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="Y6:AA6"/>
+    <mergeCell ref="T7:W7"/>
+    <mergeCell ref="X7:AA7"/>
+    <mergeCell ref="T8:X9"/>
+    <mergeCell ref="Y8:AA8"/>
+    <mergeCell ref="Y9:AA9"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="AR7:AU7"/>
+    <mergeCell ref="AV7:AY7"/>
+    <mergeCell ref="AR8:AV9"/>
+    <mergeCell ref="AW8:AY8"/>
+    <mergeCell ref="AW9:AY9"/>
+    <mergeCell ref="AJ5:AN6"/>
+    <mergeCell ref="AO5:AQ5"/>
+    <mergeCell ref="AO6:AQ6"/>
+    <mergeCell ref="AJ7:AM7"/>
+    <mergeCell ref="AN7:AQ7"/>
+    <mergeCell ref="AJ8:AN9"/>
+    <mergeCell ref="AO8:AQ8"/>
+    <mergeCell ref="AO9:AQ9"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:K4"/>
+    <mergeCell ref="L4:S4"/>
+    <mergeCell ref="T4:AA4"/>
+    <mergeCell ref="AB4:AI4"/>
+    <mergeCell ref="AJ4:AQ4"/>
+    <mergeCell ref="AR5:AV6"/>
+    <mergeCell ref="AW5:AY5"/>
+    <mergeCell ref="AW6:AY6"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="AB5:AF6"/>
+    <mergeCell ref="AG5:AI5"/>
+    <mergeCell ref="AG6:AI6"/>
+    <mergeCell ref="A5:C6"/>
+    <mergeCell ref="D5:H6"/>
+    <mergeCell ref="L5:P6"/>
+    <mergeCell ref="A3:AY3"/>
+    <mergeCell ref="X31:Y32"/>
+    <mergeCell ref="T33:W34"/>
+    <mergeCell ref="X33:Y34"/>
+    <mergeCell ref="A33:C34"/>
+    <mergeCell ref="D28:K28"/>
+    <mergeCell ref="L28:S28"/>
+    <mergeCell ref="T28:AA28"/>
+    <mergeCell ref="AB28:AI28"/>
+    <mergeCell ref="AJ28:AQ28"/>
+    <mergeCell ref="AR28:AY28"/>
+    <mergeCell ref="AB29:AE30"/>
+    <mergeCell ref="Z29:AA29"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C30"/>
+    <mergeCell ref="D29:G30"/>
+    <mergeCell ref="H29:I30"/>
+    <mergeCell ref="A27:AY27"/>
+    <mergeCell ref="A31:C32"/>
+    <mergeCell ref="D31:G32"/>
+    <mergeCell ref="H31:I32"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="L31:O32"/>
+    <mergeCell ref="AR4:AY4"/>
+    <mergeCell ref="D37:K37"/>
+    <mergeCell ref="A36:AY36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="AP33:AQ33"/>
+    <mergeCell ref="AR33:AU34"/>
+    <mergeCell ref="AV33:AW34"/>
+    <mergeCell ref="AX33:AY33"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="R34:S34"/>
+    <mergeCell ref="Z34:AA34"/>
+    <mergeCell ref="AH34:AI34"/>
+    <mergeCell ref="AX34:AY34"/>
+    <mergeCell ref="Z33:AA33"/>
+    <mergeCell ref="AB33:AE34"/>
+    <mergeCell ref="AF33:AG34"/>
+    <mergeCell ref="AH33:AI33"/>
+    <mergeCell ref="AJ33:AM34"/>
+    <mergeCell ref="AN33:AO34"/>
+    <mergeCell ref="D33:G34"/>
+    <mergeCell ref="H33:I34"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="L33:O34"/>
+    <mergeCell ref="P33:Q34"/>
+    <mergeCell ref="R33:S33"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="D40:K40"/>
+    <mergeCell ref="L40:S40"/>
+    <mergeCell ref="T40:AA40"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="Q39:S39"/>
+    <mergeCell ref="Y39:AA39"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="Q38:S38"/>
+    <mergeCell ref="Y38:AA38"/>
+    <mergeCell ref="A38:C39"/>
+    <mergeCell ref="D38:G39"/>
+    <mergeCell ref="L38:O39"/>
+    <mergeCell ref="T38:W39"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:O30"/>
+    <mergeCell ref="P29:Q30"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="T29:W30"/>
+    <mergeCell ref="X29:Y30"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="R32:S32"/>
+    <mergeCell ref="Z32:AA32"/>
+    <mergeCell ref="Z31:AA31"/>
+    <mergeCell ref="P31:Q32"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="T31:W32"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="Z30:AA30"/>
+    <mergeCell ref="AH30:AI30"/>
+    <mergeCell ref="AP30:AQ30"/>
+    <mergeCell ref="AX30:AY30"/>
+    <mergeCell ref="AF29:AG30"/>
+    <mergeCell ref="AH29:AI29"/>
+    <mergeCell ref="AJ29:AM30"/>
+    <mergeCell ref="AN29:AO30"/>
+    <mergeCell ref="AP29:AQ29"/>
+    <mergeCell ref="AR29:AU30"/>
+    <mergeCell ref="AC43:AR43"/>
+    <mergeCell ref="AC55:AR55"/>
+    <mergeCell ref="AQ12:BE12"/>
+    <mergeCell ref="Z12:AN12"/>
+    <mergeCell ref="AW38:AY38"/>
+    <mergeCell ref="AO39:AQ39"/>
+    <mergeCell ref="AW39:AY39"/>
+    <mergeCell ref="AV29:AW30"/>
+    <mergeCell ref="AX29:AY29"/>
+    <mergeCell ref="AP34:AQ34"/>
+    <mergeCell ref="AP31:AQ31"/>
+    <mergeCell ref="AR31:AU32"/>
+    <mergeCell ref="AV31:AW32"/>
+    <mergeCell ref="AX31:AY31"/>
+    <mergeCell ref="AZ37:BF37"/>
+    <mergeCell ref="AZ40:BF40"/>
+    <mergeCell ref="AH32:AI32"/>
+    <mergeCell ref="AP32:AQ32"/>
+    <mergeCell ref="AX32:AY32"/>
+    <mergeCell ref="AB31:AE32"/>
+    <mergeCell ref="AF31:AG32"/>
+    <mergeCell ref="AH31:AI31"/>
+    <mergeCell ref="AJ31:AM32"/>
+    <mergeCell ref="AN31:AO32"/>
     <mergeCell ref="B12:P12"/>
     <mergeCell ref="S1:AN2"/>
     <mergeCell ref="A41:C41"/>
@@ -22183,195 +22371,6 @@
     <mergeCell ref="AG38:AI38"/>
     <mergeCell ref="AO38:AQ38"/>
     <mergeCell ref="J30:K30"/>
-    <mergeCell ref="AC43:AR43"/>
-    <mergeCell ref="AC55:AR55"/>
-    <mergeCell ref="AQ12:BE12"/>
-    <mergeCell ref="Z12:AN12"/>
-    <mergeCell ref="AW38:AY38"/>
-    <mergeCell ref="AO39:AQ39"/>
-    <mergeCell ref="AW39:AY39"/>
-    <mergeCell ref="AV29:AW30"/>
-    <mergeCell ref="AX29:AY29"/>
-    <mergeCell ref="AP34:AQ34"/>
-    <mergeCell ref="AP31:AQ31"/>
-    <mergeCell ref="AR31:AU32"/>
-    <mergeCell ref="AV31:AW32"/>
-    <mergeCell ref="AX31:AY31"/>
-    <mergeCell ref="AZ37:BF37"/>
-    <mergeCell ref="AZ40:BF40"/>
-    <mergeCell ref="AH32:AI32"/>
-    <mergeCell ref="AP32:AQ32"/>
-    <mergeCell ref="AX32:AY32"/>
-    <mergeCell ref="AB31:AE32"/>
-    <mergeCell ref="AF31:AG32"/>
-    <mergeCell ref="AH31:AI31"/>
-    <mergeCell ref="AJ31:AM32"/>
-    <mergeCell ref="AN31:AO32"/>
-    <mergeCell ref="AH30:AI30"/>
-    <mergeCell ref="AP30:AQ30"/>
-    <mergeCell ref="AX30:AY30"/>
-    <mergeCell ref="AF29:AG30"/>
-    <mergeCell ref="AH29:AI29"/>
-    <mergeCell ref="AJ29:AM30"/>
-    <mergeCell ref="AN29:AO30"/>
-    <mergeCell ref="AP29:AQ29"/>
-    <mergeCell ref="AR29:AU30"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:O30"/>
-    <mergeCell ref="P29:Q30"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="T29:W30"/>
-    <mergeCell ref="X29:Y30"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="R32:S32"/>
-    <mergeCell ref="Z32:AA32"/>
-    <mergeCell ref="Z31:AA31"/>
-    <mergeCell ref="P31:Q32"/>
-    <mergeCell ref="R31:S31"/>
-    <mergeCell ref="T31:W32"/>
-    <mergeCell ref="R30:S30"/>
-    <mergeCell ref="Z30:AA30"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="D40:K40"/>
-    <mergeCell ref="L40:S40"/>
-    <mergeCell ref="T40:AA40"/>
-    <mergeCell ref="I39:K39"/>
-    <mergeCell ref="Q39:S39"/>
-    <mergeCell ref="Y39:AA39"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="Q38:S38"/>
-    <mergeCell ref="Y38:AA38"/>
-    <mergeCell ref="A38:C39"/>
-    <mergeCell ref="D38:G39"/>
-    <mergeCell ref="L38:O39"/>
-    <mergeCell ref="T38:W39"/>
-    <mergeCell ref="D37:K37"/>
-    <mergeCell ref="A36:AY36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="AP33:AQ33"/>
-    <mergeCell ref="AR33:AU34"/>
-    <mergeCell ref="AV33:AW34"/>
-    <mergeCell ref="AX33:AY33"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="R34:S34"/>
-    <mergeCell ref="Z34:AA34"/>
-    <mergeCell ref="AH34:AI34"/>
-    <mergeCell ref="AX34:AY34"/>
-    <mergeCell ref="Z33:AA33"/>
-    <mergeCell ref="AB33:AE34"/>
-    <mergeCell ref="AF33:AG34"/>
-    <mergeCell ref="AH33:AI33"/>
-    <mergeCell ref="AJ33:AM34"/>
-    <mergeCell ref="AN33:AO34"/>
-    <mergeCell ref="D33:G34"/>
-    <mergeCell ref="H33:I34"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="L33:O34"/>
-    <mergeCell ref="P33:Q34"/>
-    <mergeCell ref="R33:S33"/>
-    <mergeCell ref="A3:AY3"/>
-    <mergeCell ref="X31:Y32"/>
-    <mergeCell ref="T33:W34"/>
-    <mergeCell ref="X33:Y34"/>
-    <mergeCell ref="A33:C34"/>
-    <mergeCell ref="D28:K28"/>
-    <mergeCell ref="L28:S28"/>
-    <mergeCell ref="T28:AA28"/>
-    <mergeCell ref="AB28:AI28"/>
-    <mergeCell ref="AJ28:AQ28"/>
-    <mergeCell ref="AR28:AY28"/>
-    <mergeCell ref="AB29:AE30"/>
-    <mergeCell ref="Z29:AA29"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C30"/>
-    <mergeCell ref="D29:G30"/>
-    <mergeCell ref="H29:I30"/>
-    <mergeCell ref="A27:AY27"/>
-    <mergeCell ref="A31:C32"/>
-    <mergeCell ref="D31:G32"/>
-    <mergeCell ref="H31:I32"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="L31:O32"/>
-    <mergeCell ref="AR4:AY4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:K4"/>
-    <mergeCell ref="L4:S4"/>
-    <mergeCell ref="T4:AA4"/>
-    <mergeCell ref="AB4:AI4"/>
-    <mergeCell ref="AJ4:AQ4"/>
-    <mergeCell ref="AR5:AV6"/>
-    <mergeCell ref="AW5:AY5"/>
-    <mergeCell ref="AW6:AY6"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="AB5:AF6"/>
-    <mergeCell ref="AG5:AI5"/>
-    <mergeCell ref="AG6:AI6"/>
-    <mergeCell ref="A5:C6"/>
-    <mergeCell ref="D5:H6"/>
-    <mergeCell ref="L5:P6"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="AR7:AU7"/>
-    <mergeCell ref="AV7:AY7"/>
-    <mergeCell ref="AR8:AV9"/>
-    <mergeCell ref="AW8:AY8"/>
-    <mergeCell ref="AW9:AY9"/>
-    <mergeCell ref="AJ5:AN6"/>
-    <mergeCell ref="AO5:AQ5"/>
-    <mergeCell ref="AO6:AQ6"/>
-    <mergeCell ref="AJ7:AM7"/>
-    <mergeCell ref="AN7:AQ7"/>
-    <mergeCell ref="AJ8:AN9"/>
-    <mergeCell ref="AO8:AQ8"/>
-    <mergeCell ref="AO9:AQ9"/>
-    <mergeCell ref="AZ4:BF4"/>
-    <mergeCell ref="AZ28:BF28"/>
-    <mergeCell ref="AB7:AE7"/>
-    <mergeCell ref="AF7:AI7"/>
-    <mergeCell ref="AB8:AF9"/>
-    <mergeCell ref="AG8:AI8"/>
-    <mergeCell ref="AG9:AI9"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="D8:H9"/>
-    <mergeCell ref="T5:X6"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="Y6:AA6"/>
-    <mergeCell ref="T7:W7"/>
-    <mergeCell ref="X7:AA7"/>
-    <mergeCell ref="T8:X9"/>
-    <mergeCell ref="Y8:AA8"/>
-    <mergeCell ref="Y9:AA9"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="BB1:BF1"/>
-    <mergeCell ref="AW1:BA1"/>
-    <mergeCell ref="P7:S7"/>
-    <mergeCell ref="L8:P9"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="A1:P2"/>
-    <mergeCell ref="AZ41:BF41"/>
-    <mergeCell ref="AZ8:BF8"/>
-    <mergeCell ref="AZ9:BF9"/>
-    <mergeCell ref="BA10:BB10"/>
-    <mergeCell ref="BD5:BF5"/>
-    <mergeCell ref="BD6:BF6"/>
-    <mergeCell ref="BD7:BF7"/>
-    <mergeCell ref="BA7:BC7"/>
-    <mergeCell ref="BA6:BC6"/>
-    <mergeCell ref="AZ38:BF39"/>
-    <mergeCell ref="AZ5:BC5"/>
-    <mergeCell ref="AZ29:BF29"/>
-    <mergeCell ref="AZ30:BF30"/>
-    <mergeCell ref="AZ31:BF31"/>
-    <mergeCell ref="AZ32:BF32"/>
-    <mergeCell ref="AZ33:BF33"/>
-    <mergeCell ref="AZ34:BF34"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -22389,8 +22388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AC58"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Z6" sqref="Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -22401,53 +22400,53 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:29">
-      <c r="C2" s="183" t="s">
+      <c r="C2" s="182" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="183"/>
-      <c r="E2" s="183"/>
-      <c r="F2" s="183" t="s">
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="182" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="183"/>
-      <c r="H2" s="183"/>
-      <c r="I2" s="183" t="s">
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="183"/>
-      <c r="K2" s="183"/>
-      <c r="L2" s="183" t="s">
+      <c r="J2" s="182"/>
+      <c r="K2" s="182"/>
+      <c r="L2" s="182" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="183"/>
-      <c r="N2" s="183"/>
-      <c r="O2" s="183" t="s">
+      <c r="M2" s="182"/>
+      <c r="N2" s="182"/>
+      <c r="O2" s="182" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="183"/>
-      <c r="Q2" s="183"/>
-      <c r="R2" s="183" t="s">
+      <c r="P2" s="182"/>
+      <c r="Q2" s="182"/>
+      <c r="R2" s="182" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="183"/>
-      <c r="T2" s="183"/>
-      <c r="U2" s="183" t="s">
+      <c r="S2" s="182"/>
+      <c r="T2" s="182"/>
+      <c r="U2" s="182" t="s">
         <v>10</v>
       </c>
-      <c r="V2" s="183"/>
-      <c r="W2" s="183"/>
-      <c r="X2" s="183" t="s">
+      <c r="V2" s="182"/>
+      <c r="W2" s="182"/>
+      <c r="X2" s="182" t="s">
         <v>44</v>
       </c>
-      <c r="Y2" s="183"/>
-      <c r="Z2" s="183" t="s">
-        <v>229</v>
-      </c>
-      <c r="AA2" s="183"/>
-      <c r="AB2" s="183" t="s">
-        <v>231</v>
-      </c>
-      <c r="AC2" s="183"/>
+      <c r="Y2" s="182"/>
+      <c r="Z2" s="182" t="s">
+        <v>228</v>
+      </c>
+      <c r="AA2" s="182"/>
+      <c r="AB2" s="182" t="s">
+        <v>230</v>
+      </c>
+      <c r="AC2" s="182"/>
     </row>
     <row r="3" spans="2:29">
       <c r="B3" s="2" t="s">
@@ -22520,19 +22519,19 @@
         <v>2</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="Z3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AB3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="2:29">
@@ -25203,21 +25202,21 @@
     </row>
     <row r="58" spans="2:16">
       <c r="B58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="U2:W2"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="U2:W2"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25228,8 +25227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445FA1D4-95EC-4FB6-BD55-26BADBF87923}">
   <dimension ref="B2:AL51"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -25564,12 +25563,14 @@
         <v>40</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="J25" s="2"/>
+      <c r="J25" s="2" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="26" spans="2:10">
       <c r="B26" s="14" t="str">
@@ -26434,8 +26435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371172C4-9091-47C9-8DCD-1C2FDA8BA0C3}">
   <dimension ref="A1:BW93"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="AY46" workbookViewId="0">
+      <selection activeCell="BP62" sqref="BP62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>

</xml_diff>